<commit_message>
removed 'tags' from data_frame
</commit_message>
<xml_diff>
--- a/videoInformation.xlsx
+++ b/videoInformation.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H133"/>
+  <dimension ref="A1:G133"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,25 +446,20 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>tags</t>
+          <t>duration</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>duration</t>
+          <t>publised_date</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>publised_date</t>
+          <t>like_count</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>like_count</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>views_count</t>
         </is>
@@ -484,27 +479,22 @@
           <t>What is Machine Learning? | 100 Days of Machine Learning</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>['machine learning tutorial', 'machine learning course', 'machine learning python', 'machine learning algorithms', 'machine learning explained', 'machine learning algorithms for data science', 'what is machine learning', 'what is machine learning in hindi', 'machine learning basics for beginners', 'end to end machine learning', 'What is machine learning with example?', 'Machine learning introduction', 'deep learning', 'campusx', 'machine learning', 'nitish singh campusx', 'nitish sir campusx']</t>
-        </is>
-      </c>
-      <c r="E2" t="n">
+      <c r="D2" t="n">
         <v>1200</v>
       </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>2021-03-13T16:15:53Z</t>
+        </is>
+      </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>2021-03-13T16:15:53Z</t>
+          <t>8993</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>8987</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>813718</t>
+          <t>814498</t>
         </is>
       </c>
     </row>
@@ -522,27 +512,22 @@
           <t>AI Vs ML Vs DL for Beginners in Hindi</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>['ai vs ml vs dl', 'artificial intelligence vs machine learning', 'ai vs ml vs dl vs data science', 'artificial intelligence in hindi', 'machine learning vs ai', 'deep learning vs machine learning', 'ai vs ml', 'what is ai', 'what is ml', 'what is machine learning', 'machine learning in hindi', 'machine learning with python', 'ai vs ml vs ml in hindi', 'ai vs ml vs dl for beginners', 'campusx', 'nitish sir campusx', '100 days of machine learning', 'machine learning full course', 'data science in hindi']</t>
-        </is>
-      </c>
-      <c r="E3" t="n">
+      <c r="D3" t="n">
         <v>962</v>
       </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>2021-03-15T16:28:35Z</t>
+        </is>
+      </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>2021-03-15T16:28:35Z</t>
+          <t>4072</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>4069</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>151963</t>
+          <t>152105</t>
         </is>
       </c>
     </row>
@@ -560,27 +545,22 @@
           <t>Types of Machine Learning for Beginners | Types of Machine learning in Hindi | Types of ML in Depth</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>['types of machine learning', 'supervised learning in artificial intelligence', 'Types of Machine Learning for Beginners', 'Types of Machine learning in Hindi', 'supervised vs unsupervised machine learning', 'supervised vs unsupervised vs reinforcement learning', 'supervised vs unsupervised learning examples', 'supervised vs unsupervised learning algorithms', 'supervised vs unsupervised learning vs semi-supervised learning', 'campusx', 'nitish sir campusx', '100 days of machine learning']</t>
-        </is>
-      </c>
-      <c r="E4" t="n">
+      <c r="D4" t="n">
         <v>1662</v>
       </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>2021-03-16T13:49:16Z</t>
+        </is>
+      </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>2021-03-16T13:49:16Z</t>
+          <t>4476</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>4472</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>182898</t>
+          <t>183054</t>
         </is>
       </c>
     </row>
@@ -598,27 +578,22 @@
           <t>Batch Machine Learning | Offline Vs Online Learning | Machine Learning Types</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>['batch machine learning', 'online machine learning', 'types of machine learning', 'online learning', 'offline learning', 'batch learning vs online learning', 'campusx', 'nitish singh campusx', 'machine learning in urdu', 'machine learning tutorial', '100 days of machine learning', 'machine learning course', 'nitish sir campusx', 'machine learning full course', 'machine learning end to end', 'data science full course', 'data science in hindi', 'machine learning in hindi', 'machine learning for beginners']</t>
-        </is>
-      </c>
-      <c r="E5" t="n">
+      <c r="D5" t="n">
         <v>688</v>
       </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>2021-03-17T14:13:41Z</t>
+        </is>
+      </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>2021-03-17T14:13:41Z</t>
+          <t>2683</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>2680</t>
-        </is>
-      </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>120447</t>
+          <t>120567</t>
         </is>
       </c>
     </row>
@@ -636,27 +611,22 @@
           <t>Online Machine Learning | Online Learning | Online Vs Offline Machine Learning</t>
         </is>
       </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>['online machine learning', 'batch machine learning', 'types of machine learning', 'online vs batch machine learning', 'machine learning playlist', 'machine learning course', 'machine learning tutorial', 'machine learning for beginners', 'online vs offline learning', 'campusx', 'nitish sir campusx', '100 days of machine learning', 'machine learning full course', 'machine learning end to end', 'data science full course', 'data science in hindi', 'machine learning in hindi', 'online learning']</t>
-        </is>
-      </c>
-      <c r="E6" t="n">
+      <c r="D6" t="n">
         <v>1168</v>
       </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>2021-03-18T12:41:31Z</t>
+        </is>
+      </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>2021-03-18T12:41:31Z</t>
+          <t>3267</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>3266</t>
-        </is>
-      </c>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t>103855</t>
+          <t>103930</t>
         </is>
       </c>
     </row>
@@ -674,27 +644,22 @@
           <t>Instance-Based Vs Model-Based Learning | Types of Machine Learning</t>
         </is>
       </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>['instance based learning', 'instance based machine learning', 'instance-based machine learning', 'instance-based ml', 'model-based machine learning', 'model based machine learning', 'model based learning', 'model-based learning', 'model-based ml', 'instance-based vs model-based', 'instance based vs model based', 'machine learning tutorial', 'machine learning types', 'machine learning playlist', 'campusx', 'Instance-Based Vs Model-Based Learning', 'Types of Machine Learning', 'nitish sir campusx']</t>
-        </is>
-      </c>
-      <c r="E7" t="n">
+      <c r="D7" t="n">
         <v>1004</v>
       </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>2021-03-19T13:34:29Z</t>
+        </is>
+      </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>2021-03-19T13:34:29Z</t>
+          <t>2800</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>2797</t>
-        </is>
-      </c>
-      <c r="H7" t="inlineStr">
-        <is>
-          <t>96624</t>
+          <t>96692</t>
         </is>
       </c>
     </row>
@@ -712,27 +677,22 @@
           <t>Challenges in Machine Learning | Problems in Machine Learning</t>
         </is>
       </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>['challenges of machine learning', 'challenges of ml', '100 days of machine learning', 'campusx', 'challenges for machine learning', 'machine learning in industry', 'intuitive machine learning', 'machine learning playlist', 'data science full course in hindi', 'machine learning course for beginners', 'machine learning end to end', 'data science full course', 'data science in hindi', 'machine learning in hindi', 'data science for beginners', 'challenges in machine learning', 'problems in machine learning']</t>
-        </is>
-      </c>
-      <c r="E8" t="n">
+      <c r="D8" t="n">
         <v>1420</v>
       </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>2021-03-20T14:09:26Z</t>
+        </is>
+      </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>2021-03-20T14:09:26Z</t>
+          <t>2984</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>2981</t>
-        </is>
-      </c>
-      <c r="H8" t="inlineStr">
-        <is>
-          <t>85409</t>
+          <t>85501</t>
         </is>
       </c>
     </row>
@@ -750,27 +710,22 @@
           <t>Application of Machine Learning | Real Life Machine Learning Applications</t>
         </is>
       </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>['machine learning applications', 'real-life machine learning applications', 'machine learning applications example', 'machine learning based products', 'machile learning for beginners', 'top 10 applications of machine learning', 'campusx', 'data science full course', 'machine learning full course', 'data science full course in hindi', 'machine learning full course in hindi', 'how companies use machine learning', 'practical uses of data science', 'examples of data science', 'intuitive data science']</t>
-        </is>
-      </c>
-      <c r="E9" t="n">
+      <c r="D9" t="n">
         <v>1742</v>
       </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>2021-03-22T14:14:44Z</t>
+        </is>
+      </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>2021-03-22T14:14:44Z</t>
+          <t>3585</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>3582</t>
-        </is>
-      </c>
-      <c r="H9" t="inlineStr">
-        <is>
-          <t>72170</t>
+          <t>72238</t>
         </is>
       </c>
     </row>
@@ -788,27 +743,22 @@
           <t>Machine Learning Development Life Cycle | MLDLC in Data Science</t>
         </is>
       </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>['machine learning life cycle', 'development of machine learning', 'life cycle of machine learning in hindi', 'ml life cycle', 'complete machine learning course', 'campusx', 'nitish sir campusx', '100 days of machine learning', 'machine learning full course', 'machine learning end to end', 'data science full course', 'data science in hindi', 'machine learning in hindi', 'data science for beginners', 'machine learning for beginners', 'Machine Learning Development Life Cycle', 'MLDLC in Data Science']</t>
-        </is>
-      </c>
-      <c r="E10" t="n">
+      <c r="D10" t="n">
         <v>1513</v>
       </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>2021-03-23T14:44:09Z</t>
+        </is>
+      </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>2021-03-23T14:44:09Z</t>
+          <t>3084</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>3080</t>
-        </is>
-      </c>
-      <c r="H10" t="inlineStr">
-        <is>
-          <t>86879</t>
+          <t>86963</t>
         </is>
       </c>
     </row>
@@ -826,27 +776,22 @@
           <t>Data Engineer Vs Data Analyst Vs Data Scientist Vs ML Engineer | Data Science Job Roles</t>
         </is>
       </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>['data engineer vs data analyst', 'data scientist vs data analyst', 'what is data engineering', 'data engineer vs data scientist', 'data analyst vs data engineer', 'data engineer vs data analyst vs data scientist', 'Data Engineer V Data Analyst V Data Scientist V ML Engineer', 'Data Science Job Roles', 'ml engineer vs data scientist', 'campusx', 'nitish sir campusx', '100 days of machine learning', 'machine learning end to end', 'machine learning in hindi', 'data science for beginners']</t>
-        </is>
-      </c>
-      <c r="E11" t="n">
+      <c r="D11" t="n">
         <v>1583</v>
       </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>2021-03-24T12:49:59Z</t>
+        </is>
+      </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>2021-03-24T12:49:59Z</t>
+          <t>2597</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>2596</t>
-        </is>
-      </c>
-      <c r="H11" t="inlineStr">
-        <is>
-          <t>67370</t>
+          <t>67414</t>
         </is>
       </c>
     </row>
@@ -864,27 +809,22 @@
           <t>What are Tensors | Tensor In-depth Explanation | Tensor in Machine Learning</t>
         </is>
       </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>['machine learning tensor', 'deep learning tensor', 'vector tensor', 'tensor shape', 'nlp tensor', 'video tensor', 'image tensor', 'campusx', 'nitish singh campusx', '100 days of machine learning', 'machine learning full course', 'machine learning end to end', 'data science full course', 'data science in hindi', 'machine learning in hindi', 'intuitive machine learning', 'data science for beginners', 'machine learning for beginners', 'What are Tensors', 'Tensor In-depth Explanation', 'Tensor in Machine Learning']</t>
-        </is>
-      </c>
-      <c r="E12" t="n">
+      <c r="D12" t="n">
         <v>2489</v>
       </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>2021-03-25T14:39:26Z</t>
+        </is>
+      </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>2021-03-25T14:39:26Z</t>
+          <t>4205</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>4203</t>
-        </is>
-      </c>
-      <c r="H12" t="inlineStr">
-        <is>
-          <t>126990</t>
+          <t>127103</t>
         </is>
       </c>
     </row>
@@ -902,27 +842,22 @@
           <t>Installing Anaconda For Data Science | Jupyter Notebook for Machine Learning | Google Colab for ML</t>
         </is>
       </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>['google colab vs jupyter notebook', 'installing anaconda on windows 10', 'installing jupyter notebook on windows 10', 'anaconda tutorial', 'jupyter notebook tutorial', 'google colab python', 'kaggle notebook vs colab', 'how to run python code on google colab', 'jupyter notebook vs google colab', 'google colab vs kaggle', 'campusx', 'Installing Anaconda For Data Science', 'Jupyter Notebook for Machine Learning', 'Google Colab for ML', '100 days of machine learning', 'machine learning in hindi']</t>
-        </is>
-      </c>
-      <c r="E13" t="n">
+      <c r="D13" t="n">
         <v>2226</v>
       </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>2021-03-26T15:47:45Z</t>
+        </is>
+      </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>2021-03-26T15:47:45Z</t>
+          <t>3023</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>3022</t>
-        </is>
-      </c>
-      <c r="H13" t="inlineStr">
-        <is>
-          <t>97646</t>
+          <t>97728</t>
         </is>
       </c>
     </row>
@@ -940,27 +875,22 @@
           <t>End to End Toy Project | Day 13 | 100 Days of Machine Learning</t>
         </is>
       </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>['Education', 'Engineering', 'Campus', 'Placement', 'Skills', 'Machine Learning', 'Software', 'Web Development', 'Profile Building', 'end to end machine learning project', 'machine learning toy project', 'ai ml project', 'machine learning begineers', 'ml projects in python', 'ml projects ideas', 'learn machine learning using projects']</t>
-        </is>
-      </c>
-      <c r="E14" t="n">
+      <c r="D14" t="n">
         <v>1843</v>
       </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>2021-03-27T14:30:02Z</t>
+        </is>
+      </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>2021-03-27T14:30:02Z</t>
+          <t>3278</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>3276</t>
-        </is>
-      </c>
-      <c r="H14" t="inlineStr">
-        <is>
-          <t>120324</t>
+          <t>120425</t>
         </is>
       </c>
     </row>
@@ -978,27 +908,22 @@
           <t>How to Frame a Machine Learning Problem | How to plan a Data Science Project Effectively</t>
         </is>
       </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>['how to approach any machine learning problem', 'approaching a machine learning problem from scratch', 'how to solve a machine learning problem', 'machine learning step by step', 'step by step approach for a machine learning problem', 'solving a machine learning use case', 'stepwise process for data science', 'Framing a Machine Learning Problem', 'How to plan a Data Science Project', 'campusx', 'nitish sir campusx', '100 days of machine learning', 'data science in hindi', 'machine learning in hindi']</t>
-        </is>
-      </c>
-      <c r="E15" t="n">
+      <c r="D15" t="n">
         <v>1342</v>
       </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>2021-03-29T14:30:01Z</t>
+        </is>
+      </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>2021-03-29T14:30:01Z</t>
+          <t>3075</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>3074</t>
-        </is>
-      </c>
-      <c r="H15" t="inlineStr">
-        <is>
-          <t>78522</t>
+          <t>78585</t>
         </is>
       </c>
     </row>
@@ -1016,27 +941,22 @@
           <t>Working with CSV files | Day 15 | 100 Days of Machine Learning</t>
         </is>
       </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>['Education', 'Engineering', 'Campus', 'Placement', 'Skills', 'Machine Learning', 'Software', 'Web Development', 'Profile Building', 'csv', 'csv python', 'how do i import a csv file into google colab?', 'how to read csv file in google colab', 'pandas csv to dataframe', 'pandas dataframe', 'pandas read excel', 'pandas read csv', 'read csv file in python', 'python write csv', 'pd read_csv', 'python read excel', 'pandas excel tutorial', 'pandas csv tutorial']</t>
-        </is>
-      </c>
-      <c r="E16" t="n">
+      <c r="D16" t="n">
         <v>2190</v>
       </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>2021-03-30T14:34:19Z</t>
+        </is>
+      </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>2021-03-30T14:34:19Z</t>
+          <t>3091</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>3089</t>
-        </is>
-      </c>
-      <c r="H16" t="inlineStr">
-        <is>
-          <t>100822</t>
+          <t>100894</t>
         </is>
       </c>
     </row>
@@ -1054,27 +974,22 @@
           <t>Working with JSON/SQL | Day 16 | 100 Days of Machine Learning</t>
         </is>
       </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>['Education', 'Engineering', 'Campus', 'Placement', 'Skills', 'Machine Learning', 'Software', 'Web Development', 'Profile Building', 'for json path', 'query json', 'convert json to table', 'convert table to json', 'sql json', 'sql', 'ml', 'ai', 'machine learning sql', 'load sql data', 'load from mysql database', 'load dataset', 'read from sql database']</t>
-        </is>
-      </c>
-      <c r="E17" t="n">
+      <c r="D17" t="n">
         <v>1020</v>
       </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>2021-03-31T14:30:04Z</t>
+        </is>
+      </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>2021-03-31T14:30:04Z</t>
+          <t>1952</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>1949</t>
-        </is>
-      </c>
-      <c r="H17" t="inlineStr">
-        <is>
-          <t>69105</t>
+          <t>69183</t>
         </is>
       </c>
     </row>
@@ -1092,27 +1007,22 @@
           <t>Fetching Data From an API | Day 17 | 100 Days of Machine Learning</t>
         </is>
       </c>
-      <c r="D18" t="inlineStr">
-        <is>
-          <t>['Education', 'Engineering', 'Campus', 'Placement', 'Skills', 'Machine Learning', 'Software', 'Web Development', 'Profile Building', 'extract data using api', 'how to extract data from api using python', 'extract data from api python', 'what is an api and how exactly it works', 'how to extract data using api?', 'extract data from an api', 'how to extract data through api?', 'what is application programming interface?', 'what exactly is an api?']</t>
-        </is>
-      </c>
-      <c r="E18" t="n">
+      <c r="D18" t="n">
         <v>1370</v>
       </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>2021-04-01T14:30:08Z</t>
+        </is>
+      </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>2021-04-01T14:30:08Z</t>
+          <t>3215</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>3210</t>
-        </is>
-      </c>
-      <c r="H18" t="inlineStr">
-        <is>
-          <t>106583</t>
+          <t>106642</t>
         </is>
       </c>
     </row>
@@ -1130,27 +1040,22 @@
           <t>Fetching data using Web Scraping | Day 18 | 100 Days of Machine Learning</t>
         </is>
       </c>
-      <c r="D19" t="inlineStr">
-        <is>
-          <t>['machine learning', 'ml', 'ai', 'web scraping in ml', 'web scraping in machine learning', 'data gathering', 'web scraping python', 'web scrapping', 'how to extract data from web page', 'hands-on with web scraping using python and beautifulsoup', 'data extraction for machine learning', 'learn web scraping in step by step manner', 'what is web scraping used for?', 'intro to web scraping with python and beautiful soup', 'how to get paragraph data from web page', '100 days of ml', 'machine learning for beginners']</t>
-        </is>
-      </c>
-      <c r="E19" t="n">
+      <c r="D19" t="n">
         <v>2269</v>
       </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>2021-04-02T15:12:18Z</t>
+        </is>
+      </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>2021-04-02T15:12:18Z</t>
+          <t>3440</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>3440</t>
-        </is>
-      </c>
-      <c r="H19" t="inlineStr">
-        <is>
-          <t>120075</t>
+          <t>120135</t>
         </is>
       </c>
     </row>
@@ -1168,27 +1073,22 @@
           <t>Understanding Your Data | Day 19 | 100 Days of Machine Learning</t>
         </is>
       </c>
-      <c r="D20" t="inlineStr">
-        <is>
-          <t>['Education', 'Engineering', 'Campus', 'Placement', 'Skills', 'Machine Learning', 'Software', 'Web Development', 'Profile Building', 'data leakage in data science', 'value of data', 'improve machine learning model', 'ml data', 'python pandas', 'use data in machine learning', 'data usage in ml', 'campusx', 'machine learning for beginners', 'ml', 'ai', 'machine learning']</t>
-        </is>
-      </c>
-      <c r="E20" t="n">
+      <c r="D20" t="n">
         <v>923</v>
       </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>2021-04-03T14:30:03Z</t>
+        </is>
+      </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>2021-04-03T14:30:03Z</t>
+          <t>2103</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>2101</t>
-        </is>
-      </c>
-      <c r="H20" t="inlineStr">
-        <is>
-          <t>79635</t>
+          <t>79697</t>
         </is>
       </c>
     </row>
@@ -1206,27 +1106,22 @@
           <t>EDA using Univariate Analysis | Day 20 | 100 Days of Machine Learning</t>
         </is>
       </c>
-      <c r="D21" t="inlineStr">
-        <is>
-          <t>['Education', 'Engineering', 'Campus', 'Placement', 'Skills', 'Machine Learning', 'Software', 'Web Development', 'Profile Building', 'exploratory data analysis', 'what is eda', 'exploratory data analysis pandas', 'objective of eda', 'eda in python', 'eda use case', 'univariate eda', 'different eda techniques', 'eda in machine learning', 'eda in ml', 'ml for beginners', '100 days of machine learning']</t>
-        </is>
-      </c>
-      <c r="E21" t="n">
+      <c r="D21" t="n">
         <v>1831</v>
       </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>2021-04-05T14:30:00Z</t>
+        </is>
+      </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>2021-04-05T14:30:00Z</t>
+          <t>2735</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>2734</t>
-        </is>
-      </c>
-      <c r="H21" t="inlineStr">
-        <is>
-          <t>112028</t>
+          <t>112125</t>
         </is>
       </c>
     </row>
@@ -1244,27 +1139,22 @@
           <t>EDA using Bivariate and Multivariate Analysis | Day 21 | 100 Days of Machine Learning</t>
         </is>
       </c>
-      <c r="D22" t="inlineStr">
-        <is>
-          <t>['Education', 'Engineering', 'Campus', 'Placement', 'Skills', 'Machine Learning', 'Software', 'Web Development', 'Profile Building']</t>
-        </is>
-      </c>
-      <c r="E22" t="n">
+      <c r="D22" t="n">
         <v>2283</v>
       </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>2021-04-06T14:30:00Z</t>
+        </is>
+      </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>2021-04-06T14:30:00Z</t>
+          <t>2456</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>2455</t>
-        </is>
-      </c>
-      <c r="H22" t="inlineStr">
-        <is>
-          <t>92976</t>
+          <t>93061</t>
         </is>
       </c>
     </row>
@@ -1282,27 +1172,22 @@
           <t>Pandas Profiling | Day 22 | 100 Days of Machine Learning</t>
         </is>
       </c>
-      <c r="D23" t="inlineStr">
-        <is>
-          <t>['Education', 'Engineering', 'Campus', 'Placement', 'Skills', 'Machine Learning', 'Software', 'Web Development', 'Profile Building']</t>
-        </is>
-      </c>
-      <c r="E23" t="n">
+      <c r="D23" t="n">
         <v>784</v>
       </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>2021-04-07T14:30:01Z</t>
+        </is>
+      </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>2021-04-07T14:30:01Z</t>
+          <t>2093</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>2093</t>
-        </is>
-      </c>
-      <c r="H23" t="inlineStr">
-        <is>
-          <t>64820</t>
+          <t>64876</t>
         </is>
       </c>
     </row>
@@ -1320,27 +1205,22 @@
           <t>What is Feature Engineering | Day 23 | 100 Days of Machine Learning</t>
         </is>
       </c>
-      <c r="D24" t="inlineStr">
-        <is>
-          <t>['Education', 'Engineering', 'Campus', 'Placement', 'Skills', 'Machine Learning', 'Software', 'Web Development', 'Profile Building']</t>
-        </is>
-      </c>
-      <c r="E24" t="n">
+      <c r="D24" t="n">
         <v>1492</v>
       </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>2021-04-08T14:43:42Z</t>
+        </is>
+      </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>2021-04-08T14:43:42Z</t>
+          <t>3030</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>3030</t>
-        </is>
-      </c>
-      <c r="H24" t="inlineStr">
-        <is>
-          <t>130088</t>
+          <t>130207</t>
         </is>
       </c>
     </row>
@@ -1358,27 +1238,22 @@
           <t>Feature Scaling - Standardization | Day 24 | 100 Days of Machine Learning</t>
         </is>
       </c>
-      <c r="D25" t="inlineStr">
-        <is>
-          <t>['Education', 'Engineering', 'Campus', 'Placement', 'Skills', 'Machine Learning', 'Software', 'Web Development', 'Profile Building']</t>
-        </is>
-      </c>
-      <c r="E25" t="n">
+      <c r="D25" t="n">
         <v>1958</v>
       </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>2021-04-09T14:32:00Z</t>
+        </is>
+      </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>2021-04-09T14:32:00Z</t>
+          <t>3304</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>3302</t>
-        </is>
-      </c>
-      <c r="H25" t="inlineStr">
-        <is>
-          <t>126039</t>
+          <t>126114</t>
         </is>
       </c>
     </row>
@@ -1396,27 +1271,22 @@
           <t>Feature Scaling - Normalization | MinMaxScaling | MaxAbsScaling | RobustScaling</t>
         </is>
       </c>
-      <c r="D26" t="inlineStr">
-        <is>
-          <t>['Education', 'Engineering', 'Campus', 'Placement', 'Skills', 'Machine Learning', 'Software', 'Web Development', 'Profile Building']</t>
-        </is>
-      </c>
-      <c r="E26" t="n">
+      <c r="D26" t="n">
         <v>1411</v>
       </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>2021-04-10T14:30:04Z</t>
+        </is>
+      </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>2021-04-10T14:30:04Z</t>
+          <t>2497</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>2495</t>
-        </is>
-      </c>
-      <c r="H26" t="inlineStr">
-        <is>
-          <t>92213</t>
+          <t>92298</t>
         </is>
       </c>
     </row>
@@ -1434,27 +1304,22 @@
           <t>Encoding Categorical Data | Ordinal Encoding | Label Encoding</t>
         </is>
       </c>
-      <c r="D27" t="inlineStr">
-        <is>
-          <t>['Education', 'Engineering', 'Campus', 'Placement', 'Skills', 'Machine Learning', 'Software', 'Web Development', 'Profile Building']</t>
-        </is>
-      </c>
-      <c r="E27" t="n">
+      <c r="D27" t="n">
         <v>1193</v>
       </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>2021-04-12T16:55:33Z</t>
+        </is>
+      </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>2021-04-12T16:55:33Z</t>
+          <t>2361</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>2360</t>
-        </is>
-      </c>
-      <c r="H27" t="inlineStr">
-        <is>
-          <t>98662</t>
+          <t>98744</t>
         </is>
       </c>
     </row>
@@ -1472,27 +1337,22 @@
           <t>One Hot Encoding | Handling Categorical Data | Day 27 | 100 Days of Machine Learning</t>
         </is>
       </c>
-      <c r="D28" t="inlineStr">
-        <is>
-          <t>['Education', 'Engineering', 'Campus', 'Placement', 'Skills', 'Machine Learning', 'Software', 'Web Development', 'Profile Building']</t>
-        </is>
-      </c>
-      <c r="E28" t="n">
+      <c r="D28" t="n">
         <v>1812</v>
       </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>2021-04-13T14:30:05Z</t>
+        </is>
+      </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>2021-04-13T14:30:05Z</t>
+          <t>2674</t>
         </is>
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>2673</t>
-        </is>
-      </c>
-      <c r="H28" t="inlineStr">
-        <is>
-          <t>107513</t>
+          <t>107602</t>
         </is>
       </c>
     </row>
@@ -1510,27 +1370,22 @@
           <t>Column Transformer in Machine Learning | How to use ColumnTransformer in Sklearn</t>
         </is>
       </c>
-      <c r="D29" t="inlineStr">
-        <is>
-          <t>['Education', 'Engineering', 'Campus', 'Placement', 'Skills', 'Machine Learning', 'Software', 'Web Development', 'Profile Building']</t>
-        </is>
-      </c>
-      <c r="E29" t="n">
+      <c r="D29" t="n">
         <v>941</v>
       </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>2021-04-14T14:30:00Z</t>
+        </is>
+      </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>2021-04-14T14:30:00Z</t>
+          <t>2333</t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>2331</t>
-        </is>
-      </c>
-      <c r="H29" t="inlineStr">
-        <is>
-          <t>90417</t>
+          <t>90468</t>
         </is>
       </c>
     </row>
@@ -1548,27 +1403,22 @@
           <t>Machine Learning Pipelines A-Z | Day 29 | 100 Days of Machine Learning</t>
         </is>
       </c>
-      <c r="D30" t="inlineStr">
-        <is>
-          <t>['Education', 'Engineering', 'Campus', 'Placement', 'Skills', 'Machine Learning', 'Software', 'Web Development', 'Profile Building']</t>
-        </is>
-      </c>
-      <c r="E30" t="n">
+      <c r="D30" t="n">
         <v>2739</v>
       </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>2021-04-15T15:00:41Z</t>
+        </is>
+      </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>2021-04-15T15:00:41Z</t>
+          <t>3552</t>
         </is>
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>3549</t>
-        </is>
-      </c>
-      <c r="H30" t="inlineStr">
-        <is>
-          <t>121793</t>
+          <t>121871</t>
         </is>
       </c>
     </row>
@@ -1586,27 +1436,22 @@
           <t>Function Transformer | Log Transform | Reciprocal Transform | Square Root Transform</t>
         </is>
       </c>
-      <c r="D31" t="inlineStr">
-        <is>
-          <t>['Education', 'Engineering', 'Campus', 'Placement', 'Skills', 'Machine Learning', 'Software', 'Web Development', 'Profile Building']</t>
-        </is>
-      </c>
-      <c r="E31" t="n">
+      <c r="D31" t="n">
         <v>1933</v>
       </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>2021-04-16T14:38:42Z</t>
+        </is>
+      </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>2021-04-16T14:38:42Z</t>
+          <t>1646</t>
         </is>
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>1644</t>
-        </is>
-      </c>
-      <c r="H31" t="inlineStr">
-        <is>
-          <t>73201</t>
+          <t>73251</t>
         </is>
       </c>
     </row>
@@ -1624,27 +1469,22 @@
           <t>Power Transformer | Box - Cox Transform | Yeo - Johnson Transform</t>
         </is>
       </c>
-      <c r="D32" t="inlineStr">
-        <is>
-          <t>['Education', 'Engineering', 'Campus', 'Placement', 'Skills', 'Machine Learning', 'Software', 'Web Development', 'Profile Building']</t>
-        </is>
-      </c>
-      <c r="E32" t="n">
+      <c r="D32" t="n">
         <v>1288</v>
       </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>2021-04-17T14:30:05Z</t>
+        </is>
+      </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>2021-04-17T14:30:05Z</t>
+          <t>1724</t>
         </is>
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>1724</t>
-        </is>
-      </c>
-      <c r="H32" t="inlineStr">
-        <is>
-          <t>57057</t>
+          <t>57078</t>
         </is>
       </c>
     </row>
@@ -1662,27 +1502,22 @@
           <t>Binning and Binarization | Discretization | Quantile Binning | KMeans Binning</t>
         </is>
       </c>
-      <c r="D33" t="inlineStr">
-        <is>
-          <t>['Education', 'Engineering', 'Campus', 'Placement', 'Skills', 'Machine Learning', 'Software', 'Web Development', 'Profile Building']</t>
-        </is>
-      </c>
-      <c r="E33" t="n">
+      <c r="D33" t="n">
         <v>2305</v>
       </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>2021-04-19T14:28:16Z</t>
+        </is>
+      </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>2021-04-19T14:28:16Z</t>
+          <t>1367</t>
         </is>
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>1366</t>
-        </is>
-      </c>
-      <c r="H33" t="inlineStr">
-        <is>
-          <t>55729</t>
+          <t>55764</t>
         </is>
       </c>
     </row>
@@ -1700,27 +1535,22 @@
           <t>Handling Mixed Variables | Feature Engineering</t>
         </is>
       </c>
-      <c r="D34" t="inlineStr">
-        <is>
-          <t>['Education', 'Engineering', 'Campus', 'Placement', 'Skills', 'Machine Learning', 'Software', 'Web Development', 'Profile Building']</t>
-        </is>
-      </c>
-      <c r="E34" t="n">
+      <c r="D34" t="n">
         <v>730</v>
       </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>2021-04-20T14:30:00Z</t>
+        </is>
+      </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>2021-04-20T14:30:00Z</t>
+          <t>1142</t>
         </is>
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>1142</t>
-        </is>
-      </c>
-      <c r="H34" t="inlineStr">
-        <is>
-          <t>37260</t>
+          <t>37296</t>
         </is>
       </c>
     </row>
@@ -1738,27 +1568,22 @@
           <t>Handling Date and Time Variables | Day 34 | 100 Days of Machine Learning</t>
         </is>
       </c>
-      <c r="D35" t="inlineStr">
-        <is>
-          <t>['Education', 'Engineering', 'Campus', 'Placement', 'Skills', 'Machine Learning', 'Software', 'Web Development', 'Profile Building']</t>
-        </is>
-      </c>
-      <c r="E35" t="n">
+      <c r="D35" t="n">
         <v>858</v>
       </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>2021-04-21T14:30:01Z</t>
+        </is>
+      </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>2021-04-21T14:30:01Z</t>
+          <t>1452</t>
         </is>
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>1452</t>
-        </is>
-      </c>
-      <c r="H35" t="inlineStr">
-        <is>
-          <t>39924</t>
+          <t>39948</t>
         </is>
       </c>
     </row>
@@ -1776,27 +1601,22 @@
           <t>Handling Missing Data | Part 1 | Complete Case Analysis</t>
         </is>
       </c>
-      <c r="D36" t="inlineStr">
-        <is>
-          <t>['Education', 'Engineering', 'Campus', 'Placement', 'Skills', 'Machine Learning', 'Software', 'Web Development', 'Profile Building']</t>
-        </is>
-      </c>
-      <c r="E36" t="n">
+      <c r="D36" t="n">
         <v>1494</v>
       </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>2021-04-22T14:30:00Z</t>
+        </is>
+      </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>2021-04-22T14:30:00Z</t>
+          <t>1758</t>
         </is>
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>1758</t>
-        </is>
-      </c>
-      <c r="H36" t="inlineStr">
-        <is>
-          <t>63823</t>
+          <t>63868</t>
         </is>
       </c>
     </row>
@@ -1814,27 +1634,22 @@
           <t>Handling missing data | Numerical Data | Simple Imputer</t>
         </is>
       </c>
-      <c r="D37" t="inlineStr">
-        <is>
-          <t>['Education', 'Engineering', 'Campus', 'Placement', 'Skills', 'Machine Learning', 'Software', 'Web Development', 'Profile Building']</t>
-        </is>
-      </c>
-      <c r="E37" t="n">
+      <c r="D37" t="n">
         <v>1881</v>
       </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>2021-04-23T14:30:13Z</t>
+        </is>
+      </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>2021-04-23T14:30:13Z</t>
+          <t>1454</t>
         </is>
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>1454</t>
-        </is>
-      </c>
-      <c r="H37" t="inlineStr">
-        <is>
-          <t>57084</t>
+          <t>57119</t>
         </is>
       </c>
     </row>
@@ -1852,27 +1667,22 @@
           <t>Handling Missing Categorical Data | Simple Imputer | Most Frequent Imputation | Missing Category Imp</t>
         </is>
       </c>
-      <c r="D38" t="inlineStr">
-        <is>
-          <t>['Education', 'Engineering', 'Campus', 'Placement', 'Skills', 'Machine Learning', 'Software', 'Web Development', 'Profile Building']</t>
-        </is>
-      </c>
-      <c r="E38" t="n">
+      <c r="D38" t="n">
         <v>814</v>
       </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>2021-04-24T14:30:10Z</t>
+        </is>
+      </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>2021-04-24T14:30:10Z</t>
+          <t>1035</t>
         </is>
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>1035</t>
-        </is>
-      </c>
-      <c r="H38" t="inlineStr">
-        <is>
-          <t>42976</t>
+          <t>43001</t>
         </is>
       </c>
     </row>
@@ -1890,27 +1700,22 @@
           <t>Missing Indicator | Random Sample Imputation | Handling Missing Data Part 4</t>
         </is>
       </c>
-      <c r="D39" t="inlineStr">
-        <is>
-          <t>['Education', 'Engineering', 'Campus', 'Placement', 'Skills', 'Machine Learning', 'Software', 'Web Development', 'Profile Building']</t>
-        </is>
-      </c>
-      <c r="E39" t="n">
+      <c r="D39" t="n">
         <v>2225</v>
       </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>2021-04-26T14:30:02Z</t>
+        </is>
+      </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>2021-04-26T14:30:02Z</t>
+          <t>1152</t>
         </is>
       </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t>1152</t>
-        </is>
-      </c>
-      <c r="H39" t="inlineStr">
-        <is>
-          <t>44337</t>
+          <t>44374</t>
         </is>
       </c>
     </row>
@@ -1928,27 +1733,22 @@
           <t>KNN Imputer | Multivariate Imputation | Handling Missing Data Part 5</t>
         </is>
       </c>
-      <c r="D40" t="inlineStr">
-        <is>
-          <t>['Education', 'Engineering', 'Campus', 'Placement', 'Skills', 'Machine Learning', 'Software', 'Web Development', 'Profile Building']</t>
-        </is>
-      </c>
-      <c r="E40" t="n">
+      <c r="D40" t="n">
         <v>1467</v>
       </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>2021-04-27T14:30:01Z</t>
+        </is>
+      </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>2021-04-27T14:30:01Z</t>
+          <t>1197</t>
         </is>
       </c>
       <c r="G40" t="inlineStr">
         <is>
-          <t>1195</t>
-        </is>
-      </c>
-      <c r="H40" t="inlineStr">
-        <is>
-          <t>47502</t>
+          <t>47530</t>
         </is>
       </c>
     </row>
@@ -1966,27 +1766,22 @@
           <t>Multivariate Imputation by Chained Equations for Missing Value | MICE Algorithm | Iterative Imputer</t>
         </is>
       </c>
-      <c r="D41" t="inlineStr">
-        <is>
-          <t>['Education', 'Engineering', 'Campus', 'Placement', 'Skills', 'Machine Learning', 'Software', 'Web Development', 'Profile Building']</t>
-        </is>
-      </c>
-      <c r="E41" t="n">
+      <c r="D41" t="n">
         <v>1111</v>
       </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>2021-04-28T14:30:01Z</t>
+        </is>
+      </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>2021-04-28T14:30:01Z</t>
+          <t>968</t>
         </is>
       </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t>966</t>
-        </is>
-      </c>
-      <c r="H41" t="inlineStr">
-        <is>
-          <t>35653</t>
+          <t>35671</t>
         </is>
       </c>
     </row>
@@ -2004,27 +1799,22 @@
           <t>What are Outliers | Outliers in Machine Learning</t>
         </is>
       </c>
-      <c r="D42" t="inlineStr">
-        <is>
-          <t>['Education', 'Engineering', 'Campus', 'Placement', 'Skills', 'Machine Learning', 'Software', 'Web Development', 'Profile Building']</t>
-        </is>
-      </c>
-      <c r="E42" t="n">
+      <c r="D42" t="n">
         <v>1027</v>
       </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>2021-04-29T14:30:11Z</t>
+        </is>
+      </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>2021-04-29T14:30:11Z</t>
+          <t>1380</t>
         </is>
       </c>
       <c r="G42" t="inlineStr">
         <is>
-          <t>1378</t>
-        </is>
-      </c>
-      <c r="H42" t="inlineStr">
-        <is>
-          <t>58909</t>
+          <t>58957</t>
         </is>
       </c>
     </row>
@@ -2042,27 +1832,22 @@
           <t>Outlier Detection and Removal using Z-score Method | Handling Outliers Part 2</t>
         </is>
       </c>
-      <c r="D43" t="inlineStr">
-        <is>
-          <t>['Education', 'Engineering', 'Campus', 'Placement', 'Skills', 'Machine Learning', 'Software', 'Web Development', 'Profile Building']</t>
-        </is>
-      </c>
-      <c r="E43" t="n">
+      <c r="D43" t="n">
         <v>1066</v>
       </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>2021-04-30T14:30:04Z</t>
+        </is>
+      </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>2021-04-30T14:30:04Z</t>
+          <t>1231</t>
         </is>
       </c>
       <c r="G43" t="inlineStr">
         <is>
-          <t>1229</t>
-        </is>
-      </c>
-      <c r="H43" t="inlineStr">
-        <is>
-          <t>51423</t>
+          <t>51449</t>
         </is>
       </c>
     </row>
@@ -2080,27 +1865,22 @@
           <t>Outlier Detection and Removal using the IQR Method | Handing Outliers Part 3</t>
         </is>
       </c>
-      <c r="D44" t="inlineStr">
-        <is>
-          <t>['Education', 'Engineering', 'Campus', 'Placement', 'Skills', 'Machine Learning', 'Software', 'Web Development', 'Profile Building']</t>
-        </is>
-      </c>
-      <c r="E44" t="n">
+      <c r="D44" t="n">
         <v>845</v>
       </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>2021-05-01T14:30:01Z</t>
+        </is>
+      </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>2021-05-01T14:30:01Z</t>
+          <t>1325</t>
         </is>
       </c>
       <c r="G44" t="inlineStr">
         <is>
-          <t>1324</t>
-        </is>
-      </c>
-      <c r="H44" t="inlineStr">
-        <is>
-          <t>55478</t>
+          <t>55510</t>
         </is>
       </c>
     </row>
@@ -2118,27 +1898,22 @@
           <t>Outlier Detection using the Percentile Method | Winsorization Technique</t>
         </is>
       </c>
-      <c r="D45" t="inlineStr">
-        <is>
-          <t>['Education', 'Engineering', 'Campus', 'Placement', 'Skills', 'Machine Learning', 'Software', 'Web Development', 'Profile Building']</t>
-        </is>
-      </c>
-      <c r="E45" t="n">
+      <c r="D45" t="n">
         <v>983</v>
       </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>2021-05-03T14:30:04Z</t>
+        </is>
+      </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>2021-05-03T14:30:04Z</t>
+          <t>1006</t>
         </is>
       </c>
       <c r="G45" t="inlineStr">
         <is>
-          <t>1004</t>
-        </is>
-      </c>
-      <c r="H45" t="inlineStr">
-        <is>
-          <t>32818</t>
+          <t>32840</t>
         </is>
       </c>
     </row>
@@ -2156,27 +1931,22 @@
           <t>Feature Construction | Feature Splitting</t>
         </is>
       </c>
-      <c r="D46" t="inlineStr">
-        <is>
-          <t>['Education', 'Engineering', 'Campus', 'Placement', 'Skills', 'Machine Learning', 'Software', 'Web Development', 'Profile Building']</t>
-        </is>
-      </c>
-      <c r="E46" t="n">
+      <c r="D46" t="n">
         <v>742</v>
       </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>2021-05-04T14:30:09Z</t>
+        </is>
+      </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>2021-05-04T14:30:09Z</t>
+          <t>933</t>
         </is>
       </c>
       <c r="G46" t="inlineStr">
         <is>
-          <t>932</t>
-        </is>
-      </c>
-      <c r="H46" t="inlineStr">
-        <is>
-          <t>33944</t>
+          <t>33955</t>
         </is>
       </c>
     </row>
@@ -2194,27 +1964,22 @@
           <t>Curse of Dimensionality</t>
         </is>
       </c>
-      <c r="D47" t="inlineStr">
-        <is>
-          <t>['Education', 'Engineering', 'Campus', 'Placement', 'Skills', 'Machine Learning', 'Software', 'Web Development', 'Profile Building']</t>
-        </is>
-      </c>
-      <c r="E47" t="n">
+      <c r="D47" t="n">
         <v>925</v>
       </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>2021-05-05T14:30:03Z</t>
+        </is>
+      </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>2021-05-05T14:30:03Z</t>
+          <t>1435</t>
         </is>
       </c>
       <c r="G47" t="inlineStr">
         <is>
-          <t>1433</t>
-        </is>
-      </c>
-      <c r="H47" t="inlineStr">
-        <is>
-          <t>50689</t>
+          <t>50718</t>
         </is>
       </c>
     </row>
@@ -2232,27 +1997,22 @@
           <t>Principle Component Analysis  (PCA) | Part 1 | Geometric Intuition</t>
         </is>
       </c>
-      <c r="D48" t="inlineStr">
-        <is>
-          <t>['Education', 'Engineering', 'Campus', 'Placement', 'Skills', 'Machine Learning', 'Software', 'Web Development', 'Profile Building']</t>
-        </is>
-      </c>
-      <c r="E48" t="n">
+      <c r="D48" t="n">
         <v>2034</v>
       </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>2021-05-06T14:30:03Z</t>
+        </is>
+      </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>2021-05-06T14:30:03Z</t>
+          <t>2094</t>
         </is>
       </c>
       <c r="G48" t="inlineStr">
         <is>
-          <t>2092</t>
-        </is>
-      </c>
-      <c r="H48" t="inlineStr">
-        <is>
-          <t>96547</t>
+          <t>96601</t>
         </is>
       </c>
     </row>
@@ -2270,27 +2030,22 @@
           <t>Principle Component Analysis (PCA) | Part 2 | Problem Formulation and Step by Step Solution</t>
         </is>
       </c>
-      <c r="D49" t="inlineStr">
-        <is>
-          <t>['Education', 'Engineering', 'Campus', 'Placement', 'Skills', 'Machine Learning', 'Software', 'Web Development', 'Profile Building']</t>
-        </is>
-      </c>
-      <c r="E49" t="n">
+      <c r="D49" t="n">
         <v>3377</v>
       </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>2021-05-07T14:30:04Z</t>
+        </is>
+      </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>2021-05-07T14:30:04Z</t>
+          <t>2020</t>
         </is>
       </c>
       <c r="G49" t="inlineStr">
         <is>
-          <t>2017</t>
-        </is>
-      </c>
-      <c r="H49" t="inlineStr">
-        <is>
-          <t>79803</t>
+          <t>79865</t>
         </is>
       </c>
     </row>
@@ -2308,27 +2063,22 @@
           <t>Principle Component Analysis(PCA) | Part 3 | Code Example and Visualization</t>
         </is>
       </c>
-      <c r="D50" t="inlineStr">
-        <is>
-          <t>['Education', 'Engineering', 'Campus', 'Placement', 'Skills', 'Machine Learning', 'Software', 'Web Development', 'Profile Building']</t>
-        </is>
-      </c>
-      <c r="E50" t="n">
+      <c r="D50" t="n">
         <v>2606</v>
       </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>2021-05-08T14:30:06Z</t>
+        </is>
+      </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>2021-05-08T14:30:06Z</t>
+          <t>1468</t>
         </is>
       </c>
       <c r="G50" t="inlineStr">
         <is>
-          <t>1467</t>
-        </is>
-      </c>
-      <c r="H50" t="inlineStr">
-        <is>
-          <t>51101</t>
+          <t>51135</t>
         </is>
       </c>
     </row>
@@ -2346,27 +2096,22 @@
           <t>Simple Linear Regression | Code + Intuition | Simplest Explanation in Hindi</t>
         </is>
       </c>
-      <c r="D51" t="inlineStr">
-        <is>
-          <t>['Education', 'Engineering', 'Campus', 'Placement', 'Skills', 'Machine Learning', 'Software', 'Web Development', 'Profile Building']</t>
-        </is>
-      </c>
-      <c r="E51" t="n">
+      <c r="D51" t="n">
         <v>2016</v>
       </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>2021-05-10T14:30:07Z</t>
+        </is>
+      </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>2021-05-10T14:30:07Z</t>
+          <t>2967</t>
         </is>
       </c>
       <c r="G51" t="inlineStr">
         <is>
-          <t>2963</t>
-        </is>
-      </c>
-      <c r="H51" t="inlineStr">
-        <is>
-          <t>154453</t>
+          <t>154565</t>
         </is>
       </c>
     </row>
@@ -2384,27 +2129,22 @@
           <t>Simple Linear Regression | Mathematical Formulation | Coding from Scratch</t>
         </is>
       </c>
-      <c r="D52" t="inlineStr">
-        <is>
-          <t>['Education', 'Engineering', 'Campus', 'Placement', 'Skills', 'Machine Learning', 'Software', 'Web Development', 'Profile Building']</t>
-        </is>
-      </c>
-      <c r="E52" t="n">
+      <c r="D52" t="n">
         <v>3211</v>
       </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>2021-05-11T14:30:06Z</t>
+        </is>
+      </c>
       <c r="F52" t="inlineStr">
         <is>
-          <t>2021-05-11T14:30:06Z</t>
+          <t>2902</t>
         </is>
       </c>
       <c r="G52" t="inlineStr">
         <is>
-          <t>2901</t>
-        </is>
-      </c>
-      <c r="H52" t="inlineStr">
-        <is>
-          <t>104193</t>
+          <t>104267</t>
         </is>
       </c>
     </row>
@@ -2422,27 +2162,22 @@
           <t>Regression Metrics | MSE, MAE &amp; RMSE | R2 Score &amp; Adjusted R2 Score</t>
         </is>
       </c>
-      <c r="D53" t="inlineStr">
-        <is>
-          <t>['Education', 'Engineering', 'Campus', 'Placement', 'Skills', 'Machine Learning', 'Software', 'Web Development', 'Profile Building']</t>
-        </is>
-      </c>
-      <c r="E53" t="n">
+      <c r="D53" t="n">
         <v>2636</v>
       </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>2021-05-13T14:30:02Z</t>
+        </is>
+      </c>
       <c r="F53" t="inlineStr">
         <is>
-          <t>2021-05-13T14:30:02Z</t>
+          <t>2609</t>
         </is>
       </c>
       <c r="G53" t="inlineStr">
         <is>
-          <t>2609</t>
-        </is>
-      </c>
-      <c r="H53" t="inlineStr">
-        <is>
-          <t>102628</t>
+          <t>102694</t>
         </is>
       </c>
     </row>
@@ -2460,27 +2195,22 @@
           <t>Multiple Linear Regression | Geometric Intuition &amp; Code</t>
         </is>
       </c>
-      <c r="D54" t="inlineStr">
-        <is>
-          <t>['Education', 'Engineering', 'Campus', 'Placement', 'Skills', 'Machine Learning', 'Software', 'Web Development', 'Profile Building']</t>
-        </is>
-      </c>
-      <c r="E54" t="n">
+      <c r="D54" t="n">
         <v>1257</v>
       </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>2021-05-14T14:30:01Z</t>
+        </is>
+      </c>
       <c r="F54" t="inlineStr">
         <is>
-          <t>2021-05-14T14:30:01Z</t>
+          <t>1889</t>
         </is>
       </c>
       <c r="G54" t="inlineStr">
         <is>
-          <t>1888</t>
-        </is>
-      </c>
-      <c r="H54" t="inlineStr">
-        <is>
-          <t>75907</t>
+          <t>75977</t>
         </is>
       </c>
     </row>
@@ -2498,27 +2228,22 @@
           <t>Multiple Linear Regression | Part 2 | Mathematical Formulation From Scratch</t>
         </is>
       </c>
-      <c r="D55" t="inlineStr">
-        <is>
-          <t>['Education', 'Engineering', 'Campus', 'Placement', 'Skills', 'Machine Learning', 'Software', 'Web Development', 'Profile Building']</t>
-        </is>
-      </c>
-      <c r="E55" t="n">
+      <c r="D55" t="n">
         <v>2891</v>
       </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>2021-05-15T14:30:07Z</t>
+        </is>
+      </c>
       <c r="F55" t="inlineStr">
         <is>
-          <t>2021-05-15T14:30:07Z</t>
+          <t>1750</t>
         </is>
       </c>
       <c r="G55" t="inlineStr">
         <is>
-          <t>1748</t>
-        </is>
-      </c>
-      <c r="H55" t="inlineStr">
-        <is>
-          <t>58771</t>
+          <t>58831</t>
         </is>
       </c>
     </row>
@@ -2536,27 +2261,22 @@
           <t>Multiple Linear Regression | Part 3 | Code From Scratch</t>
         </is>
       </c>
-      <c r="D56" t="inlineStr">
-        <is>
-          <t>['Education', 'Engineering', 'Campus', 'Placement', 'Skills', 'Machine Learning', 'Software', 'Web Development', 'Profile Building']</t>
-        </is>
-      </c>
-      <c r="E56" t="n">
+      <c r="D56" t="n">
         <v>961</v>
       </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>2021-05-17T14:30:03Z</t>
+        </is>
+      </c>
       <c r="F56" t="inlineStr">
         <is>
-          <t>2021-05-17T14:30:03Z</t>
+          <t>984</t>
         </is>
       </c>
       <c r="G56" t="inlineStr">
         <is>
-          <t>984</t>
-        </is>
-      </c>
-      <c r="H56" t="inlineStr">
-        <is>
-          <t>41588</t>
+          <t>41615</t>
         </is>
       </c>
     </row>
@@ -2574,27 +2294,22 @@
           <t>Gradient Descent From Scratch | End to End Gradient Descent | Gradient Descent Animation</t>
         </is>
       </c>
-      <c r="D57" t="inlineStr">
-        <is>
-          <t>['Gradient Descent', 'What is Gradient Descent', 'How does gradient descent works', 'Gradient descent in Machine Learning', 'Gradient descent linear regression', 'Gradient descent explained', 'Gradient descent from scratch', 'Gradient descent python', 'Gradient descent logistic regression', 'Gradient descent neural networks']</t>
-        </is>
-      </c>
-      <c r="E57" t="n">
+      <c r="D57" t="n">
         <v>7076</v>
       </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>2021-05-21T14:30:01Z</t>
+        </is>
+      </c>
       <c r="F57" t="inlineStr">
         <is>
-          <t>2021-05-21T14:30:01Z</t>
+          <t>5915</t>
         </is>
       </c>
       <c r="G57" t="inlineStr">
         <is>
-          <t>5912</t>
-        </is>
-      </c>
-      <c r="H57" t="inlineStr">
-        <is>
-          <t>161332</t>
+          <t>161453</t>
         </is>
       </c>
     </row>
@@ -2612,27 +2327,22 @@
           <t>Batch Gradient Descent with Code Demo | Simple Explanation in Hindi</t>
         </is>
       </c>
-      <c r="D58" t="inlineStr">
-        <is>
-          <t>['Education', 'Engineering', 'Campus', 'Placement', 'Skills', 'Machine Learning', 'Software', 'Web Development', 'Profile Building']</t>
-        </is>
-      </c>
-      <c r="E58" t="n">
+      <c r="D58" t="n">
         <v>3889</v>
       </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>2021-05-22T14:35:24Z</t>
+        </is>
+      </c>
       <c r="F58" t="inlineStr">
         <is>
-          <t>2021-05-22T14:35:24Z</t>
+          <t>1571</t>
         </is>
       </c>
       <c r="G58" t="inlineStr">
         <is>
-          <t>1570</t>
-        </is>
-      </c>
-      <c r="H58" t="inlineStr">
-        <is>
-          <t>58304</t>
+          <t>58357</t>
         </is>
       </c>
     </row>
@@ -2650,27 +2360,22 @@
           <t>Stochastic Gradient Descent</t>
         </is>
       </c>
-      <c r="D59" t="inlineStr">
-        <is>
-          <t>['Education', 'Engineering', 'Campus', 'Placement', 'Skills', 'Machine Learning', 'Software', 'Web Development', 'Profile Building']</t>
-        </is>
-      </c>
-      <c r="E59" t="n">
+      <c r="D59" t="n">
         <v>2975</v>
       </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>2021-05-25T14:30:06Z</t>
+        </is>
+      </c>
       <c r="F59" t="inlineStr">
         <is>
-          <t>2021-05-25T14:30:06Z</t>
+          <t>1274</t>
         </is>
       </c>
       <c r="G59" t="inlineStr">
         <is>
-          <t>1273</t>
-        </is>
-      </c>
-      <c r="H59" t="inlineStr">
-        <is>
-          <t>43474</t>
+          <t>43506</t>
         </is>
       </c>
     </row>
@@ -2688,27 +2393,22 @@
           <t>Mini-Batch Gradient Descent</t>
         </is>
       </c>
-      <c r="D60" t="inlineStr">
-        <is>
-          <t>['Education', 'Engineering', 'Campus', 'Placement', 'Skills', 'Machine Learning', 'Software', 'Web Development', 'Profile Building']</t>
-        </is>
-      </c>
-      <c r="E60" t="n">
+      <c r="D60" t="n">
         <v>1330</v>
       </c>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t>2021-05-26T14:30:12Z</t>
+        </is>
+      </c>
       <c r="F60" t="inlineStr">
         <is>
-          <t>2021-05-26T14:30:12Z</t>
+          <t>858</t>
         </is>
       </c>
       <c r="G60" t="inlineStr">
         <is>
-          <t>858</t>
-        </is>
-      </c>
-      <c r="H60" t="inlineStr">
-        <is>
-          <t>25263</t>
+          <t>25279</t>
         </is>
       </c>
     </row>
@@ -2726,27 +2426,22 @@
           <t>Polynomial Regression | Machine Learning</t>
         </is>
       </c>
-      <c r="D61" t="inlineStr">
-        <is>
-          <t>['Education', 'Engineering', 'Campus', 'Placement', 'Skills', 'Machine Learning', 'Software', 'Web Development', 'Profile Building']</t>
-        </is>
-      </c>
-      <c r="E61" t="n">
+      <c r="D61" t="n">
         <v>1606</v>
       </c>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t>2021-05-29T01:48:09Z</t>
+        </is>
+      </c>
       <c r="F61" t="inlineStr">
         <is>
-          <t>2021-05-29T01:48:09Z</t>
+          <t>1430</t>
         </is>
       </c>
       <c r="G61" t="inlineStr">
         <is>
-          <t>1428</t>
-        </is>
-      </c>
-      <c r="H61" t="inlineStr">
-        <is>
-          <t>60670</t>
+          <t>60712</t>
         </is>
       </c>
     </row>
@@ -2764,23 +2459,22 @@
           <t>Bias Variance Trade-off | Overfitting and Underfitting in Machine Learning</t>
         </is>
       </c>
-      <c r="D62" t="inlineStr"/>
-      <c r="E62" t="n">
+      <c r="D62" t="n">
         <v>485</v>
       </c>
+      <c r="E62" t="inlineStr">
+        <is>
+          <t>2020-06-05T19:54:56Z</t>
+        </is>
+      </c>
       <c r="F62" t="inlineStr">
         <is>
-          <t>2020-06-05T19:54:56Z</t>
+          <t>1561</t>
         </is>
       </c>
       <c r="G62" t="inlineStr">
         <is>
-          <t>1557</t>
-        </is>
-      </c>
-      <c r="H62" t="inlineStr">
-        <is>
-          <t>63746</t>
+          <t>63805</t>
         </is>
       </c>
     </row>
@@ -2798,27 +2492,22 @@
           <t>Ridge Regression Part 1 | Geometric Intuition and Code | Regularized Linear Models</t>
         </is>
       </c>
-      <c r="D63" t="inlineStr">
-        <is>
-          <t>['Education', 'Engineering', 'Campus', 'Placement', 'Skills', 'Machine Learning', 'Software', 'Web Development', 'Profile Building']</t>
-        </is>
-      </c>
-      <c r="E63" t="n">
+      <c r="D63" t="n">
         <v>1198</v>
       </c>
+      <c r="E63" t="inlineStr">
+        <is>
+          <t>2021-06-02T14:30:02Z</t>
+        </is>
+      </c>
       <c r="F63" t="inlineStr">
         <is>
-          <t>2021-06-02T14:30:02Z</t>
+          <t>1427</t>
         </is>
       </c>
       <c r="G63" t="inlineStr">
         <is>
-          <t>1425</t>
-        </is>
-      </c>
-      <c r="H63" t="inlineStr">
-        <is>
-          <t>77661</t>
+          <t>77738</t>
         </is>
       </c>
     </row>
@@ -2836,27 +2525,22 @@
           <t>Ridge Regression Part 2 | Mathematical Formulation &amp; Code from scratch | Regularized Linear Models</t>
         </is>
       </c>
-      <c r="D64" t="inlineStr">
-        <is>
-          <t>['Education', 'Engineering', 'Campus', 'Placement', 'Skills', 'Machine Learning', 'Software', 'Web Development', 'Profile Building']</t>
-        </is>
-      </c>
-      <c r="E64" t="n">
+      <c r="D64" t="n">
         <v>2621</v>
       </c>
+      <c r="E64" t="inlineStr">
+        <is>
+          <t>2021-06-03T14:30:05Z</t>
+        </is>
+      </c>
       <c r="F64" t="inlineStr">
         <is>
-          <t>2021-06-03T14:30:05Z</t>
+          <t>1018</t>
         </is>
       </c>
       <c r="G64" t="inlineStr">
         <is>
-          <t>1017</t>
-        </is>
-      </c>
-      <c r="H64" t="inlineStr">
-        <is>
-          <t>44054</t>
+          <t>44092</t>
         </is>
       </c>
     </row>
@@ -2874,27 +2558,22 @@
           <t>Ridge Regression Part 3 | Gradient Descent | Regularized Linear Models</t>
         </is>
       </c>
-      <c r="D65" t="inlineStr">
-        <is>
-          <t>['Education', 'Engineering', 'Campus', 'Placement', 'Skills', 'Machine Learning', 'Software', 'Web Development', 'Profile Building']</t>
-        </is>
-      </c>
-      <c r="E65" t="n">
+      <c r="D65" t="n">
         <v>1123</v>
       </c>
+      <c r="E65" t="inlineStr">
+        <is>
+          <t>2021-06-04T14:30:02Z</t>
+        </is>
+      </c>
       <c r="F65" t="inlineStr">
         <is>
-          <t>2021-06-04T14:30:02Z</t>
+          <t>747</t>
         </is>
       </c>
       <c r="G65" t="inlineStr">
         <is>
-          <t>746</t>
-        </is>
-      </c>
-      <c r="H65" t="inlineStr">
-        <is>
-          <t>28865</t>
+          <t>28886</t>
         </is>
       </c>
     </row>
@@ -2912,27 +2591,22 @@
           <t>5 Key Points - Ridge Regression | Part 4 | Regularized Linear Models</t>
         </is>
       </c>
-      <c r="D66" t="inlineStr">
-        <is>
-          <t>['Education', 'Engineering', 'Campus', 'Placement', 'Skills', 'Machine Learning', 'Software', 'Web Development', 'Profile Building']</t>
-        </is>
-      </c>
-      <c r="E66" t="n">
+      <c r="D66" t="n">
         <v>1817</v>
       </c>
+      <c r="E66" t="inlineStr">
+        <is>
+          <t>2021-06-08T08:42:26Z</t>
+        </is>
+      </c>
       <c r="F66" t="inlineStr">
         <is>
-          <t>2021-06-08T08:42:26Z</t>
+          <t>848</t>
         </is>
       </c>
       <c r="G66" t="inlineStr">
         <is>
-          <t>846</t>
-        </is>
-      </c>
-      <c r="H66" t="inlineStr">
-        <is>
-          <t>26898</t>
+          <t>26917</t>
         </is>
       </c>
     </row>
@@ -2950,27 +2624,22 @@
           <t>Lasso Regression | Intuition and Code Sample | Regularized Linear Models</t>
         </is>
       </c>
-      <c r="D67" t="inlineStr">
-        <is>
-          <t>['Education', 'Engineering', 'Campus', 'Placement', 'Skills', 'Machine Learning', 'Software', 'Web Development', 'Profile Building']</t>
-        </is>
-      </c>
-      <c r="E67" t="n">
+      <c r="D67" t="n">
         <v>1717</v>
       </c>
+      <c r="E67" t="inlineStr">
+        <is>
+          <t>2021-06-10T14:30:03Z</t>
+        </is>
+      </c>
       <c r="F67" t="inlineStr">
         <is>
-          <t>2021-06-10T14:30:03Z</t>
+          <t>893</t>
         </is>
       </c>
       <c r="G67" t="inlineStr">
         <is>
-          <t>892</t>
-        </is>
-      </c>
-      <c r="H67" t="inlineStr">
-        <is>
-          <t>35618</t>
+          <t>35644</t>
         </is>
       </c>
     </row>
@@ -2988,27 +2657,22 @@
           <t>Why Lasso Regression creates sparsity?</t>
         </is>
       </c>
-      <c r="D68" t="inlineStr">
-        <is>
-          <t>['Education', 'Engineering', 'Campus', 'Placement', 'Skills', 'Machine Learning', 'Software', 'Web Development', 'Profile Building']</t>
-        </is>
-      </c>
-      <c r="E68" t="n">
+      <c r="D68" t="n">
         <v>1470</v>
       </c>
+      <c r="E68" t="inlineStr">
+        <is>
+          <t>2021-06-11T14:30:02Z</t>
+        </is>
+      </c>
       <c r="F68" t="inlineStr">
         <is>
-          <t>2021-06-11T14:30:02Z</t>
+          <t>836</t>
         </is>
       </c>
       <c r="G68" t="inlineStr">
         <is>
-          <t>836</t>
-        </is>
-      </c>
-      <c r="H68" t="inlineStr">
-        <is>
-          <t>23460</t>
+          <t>23467</t>
         </is>
       </c>
     </row>
@@ -3026,27 +2690,22 @@
           <t>ElasticNet Regression | Intuition and Code Example | Regularized Linear Models</t>
         </is>
       </c>
-      <c r="D69" t="inlineStr">
-        <is>
-          <t>['Education', 'Engineering', 'Campus', 'Placement', 'Skills', 'Machine Learning', 'Software', 'Web Development', 'Profile Building']</t>
-        </is>
-      </c>
-      <c r="E69" t="n">
+      <c r="D69" t="n">
         <v>701</v>
       </c>
+      <c r="E69" t="inlineStr">
+        <is>
+          <t>2021-06-12T14:30:01Z</t>
+        </is>
+      </c>
       <c r="F69" t="inlineStr">
         <is>
-          <t>2021-06-12T14:30:01Z</t>
+          <t>646</t>
         </is>
       </c>
       <c r="G69" t="inlineStr">
         <is>
-          <t>646</t>
-        </is>
-      </c>
-      <c r="H69" t="inlineStr">
-        <is>
-          <t>20715</t>
+          <t>20727</t>
         </is>
       </c>
     </row>
@@ -3064,27 +2723,22 @@
           <t>Logistic Regression Part 1 | Perceptron Trick</t>
         </is>
       </c>
-      <c r="D70" t="inlineStr">
-        <is>
-          <t>['Education', 'Engineering', 'Campus', 'Placement', 'Skills', 'Machine Learning', 'Software', 'Web Development', 'Profile Building']</t>
-        </is>
-      </c>
-      <c r="E70" t="n">
+      <c r="D70" t="n">
         <v>2826</v>
       </c>
+      <c r="E70" t="inlineStr">
+        <is>
+          <t>2021-06-15T14:30:10Z</t>
+        </is>
+      </c>
       <c r="F70" t="inlineStr">
         <is>
-          <t>2021-06-15T14:30:10Z</t>
+          <t>2012</t>
         </is>
       </c>
       <c r="G70" t="inlineStr">
         <is>
-          <t>2011</t>
-        </is>
-      </c>
-      <c r="H70" t="inlineStr">
-        <is>
-          <t>113281</t>
+          <t>113359</t>
         </is>
       </c>
     </row>
@@ -3102,27 +2756,22 @@
           <t>Logistic Regression Part 2 | Perceptron Trick Code</t>
         </is>
       </c>
-      <c r="D71" t="inlineStr">
-        <is>
-          <t>['Education', 'Engineering', 'Campus', 'Placement', 'Skills', 'Machine Learning', 'Software', 'Web Development', 'Profile Building']</t>
-        </is>
-      </c>
-      <c r="E71" t="n">
+      <c r="D71" t="n">
         <v>1027</v>
       </c>
+      <c r="E71" t="inlineStr">
+        <is>
+          <t>2021-06-16T14:30:08Z</t>
+        </is>
+      </c>
       <c r="F71" t="inlineStr">
         <is>
-          <t>2021-06-16T14:30:08Z</t>
+          <t>1070</t>
         </is>
       </c>
       <c r="G71" t="inlineStr">
         <is>
-          <t>1069</t>
-        </is>
-      </c>
-      <c r="H71" t="inlineStr">
-        <is>
-          <t>46960</t>
+          <t>46997</t>
         </is>
       </c>
     </row>
@@ -3140,27 +2789,22 @@
           <t>Logistic Regression Part 3 | Sigmoid Function | 100 Days of ML</t>
         </is>
       </c>
-      <c r="D72" t="inlineStr">
-        <is>
-          <t>['Education', 'Engineering', 'Campus', 'Placement', 'Skills', 'Machine Learning', 'Software', 'Web Development', 'Profile Building']</t>
-        </is>
-      </c>
-      <c r="E72" t="n">
+      <c r="D72" t="n">
         <v>2444</v>
       </c>
+      <c r="E72" t="inlineStr">
+        <is>
+          <t>2021-06-17T14:30:04Z</t>
+        </is>
+      </c>
       <c r="F72" t="inlineStr">
         <is>
-          <t>2021-06-17T14:30:04Z</t>
+          <t>1487</t>
         </is>
       </c>
       <c r="G72" t="inlineStr">
         <is>
-          <t>1485</t>
-        </is>
-      </c>
-      <c r="H72" t="inlineStr">
-        <is>
-          <t>57790</t>
+          <t>57839</t>
         </is>
       </c>
     </row>
@@ -3178,27 +2822,22 @@
           <t>Logistic Regression Part 4 | Loss Function | Maximum Likelihood | Binary Cross Entropy</t>
         </is>
       </c>
-      <c r="D73" t="inlineStr">
-        <is>
-          <t>['Education', 'Engineering', 'Campus', 'Placement', 'Skills', 'Machine Learning', 'Software', 'Web Development', 'Profile Building']</t>
-        </is>
-      </c>
-      <c r="E73" t="n">
+      <c r="D73" t="n">
         <v>1743</v>
       </c>
+      <c r="E73" t="inlineStr">
+        <is>
+          <t>2021-06-18T14:30:04Z</t>
+        </is>
+      </c>
       <c r="F73" t="inlineStr">
         <is>
-          <t>2021-06-18T14:30:04Z</t>
+          <t>1355</t>
         </is>
       </c>
       <c r="G73" t="inlineStr">
         <is>
-          <t>1355</t>
-        </is>
-      </c>
-      <c r="H73" t="inlineStr">
-        <is>
-          <t>50187</t>
+          <t>50228</t>
         </is>
       </c>
     </row>
@@ -3216,27 +2855,22 @@
           <t>Derivative of Sigmoid Function</t>
         </is>
       </c>
-      <c r="D74" t="inlineStr">
-        <is>
-          <t>['Education', 'Engineering', 'Campus', 'Placement', 'Skills', 'Machine Learning', 'Software', 'Web Development', 'Profile Building']</t>
-        </is>
-      </c>
-      <c r="E74" t="n">
+      <c r="D74" t="n">
         <v>357</v>
       </c>
+      <c r="E74" t="inlineStr">
+        <is>
+          <t>2021-06-19T09:49:04Z</t>
+        </is>
+      </c>
       <c r="F74" t="inlineStr">
         <is>
-          <t>2021-06-19T09:49:04Z</t>
+          <t>595</t>
         </is>
       </c>
       <c r="G74" t="inlineStr">
         <is>
-          <t>595</t>
-        </is>
-      </c>
-      <c r="H74" t="inlineStr">
-        <is>
-          <t>25326</t>
+          <t>25349</t>
         </is>
       </c>
     </row>
@@ -3254,27 +2888,22 @@
           <t>Logistic Regression Part 5 | Gradient Descent &amp; Code From Scratch</t>
         </is>
       </c>
-      <c r="D75" t="inlineStr">
-        <is>
-          <t>['Education', 'Engineering', 'Campus', 'Placement', 'Skills', 'Machine Learning', 'Software', 'Web Development', 'Profile Building']</t>
-        </is>
-      </c>
-      <c r="E75" t="n">
+      <c r="D75" t="n">
         <v>2202</v>
       </c>
+      <c r="E75" t="inlineStr">
+        <is>
+          <t>2021-06-21T14:30:01Z</t>
+        </is>
+      </c>
       <c r="F75" t="inlineStr">
         <is>
-          <t>2021-06-21T14:30:01Z</t>
+          <t>1133</t>
         </is>
       </c>
       <c r="G75" t="inlineStr">
         <is>
-          <t>1131</t>
-        </is>
-      </c>
-      <c r="H75" t="inlineStr">
-        <is>
-          <t>44067</t>
+          <t>44086</t>
         </is>
       </c>
     </row>
@@ -3292,27 +2921,22 @@
           <t>Accuracy and Confusion Matrix | Type 1 and Type 2 Errors | Classification Metrics Part 1</t>
         </is>
       </c>
-      <c r="D76" t="inlineStr">
-        <is>
-          <t>['Education', 'Engineering', 'Campus', 'Placement', 'Skills', 'Machine Learning', 'Software', 'Web Development', 'Profile Building']</t>
-        </is>
-      </c>
-      <c r="E76" t="n">
+      <c r="D76" t="n">
         <v>2048</v>
       </c>
+      <c r="E76" t="inlineStr">
+        <is>
+          <t>2021-06-23T14:30:05Z</t>
+        </is>
+      </c>
       <c r="F76" t="inlineStr">
         <is>
-          <t>2021-06-23T14:30:05Z</t>
+          <t>1245</t>
         </is>
       </c>
       <c r="G76" t="inlineStr">
         <is>
-          <t>1243</t>
-        </is>
-      </c>
-      <c r="H76" t="inlineStr">
-        <is>
-          <t>58864</t>
+          <t>58905</t>
         </is>
       </c>
     </row>
@@ -3330,27 +2954,22 @@
           <t>Precision, Recall and F1 Score | Classification Metrics Part 2</t>
         </is>
       </c>
-      <c r="D77" t="inlineStr">
-        <is>
-          <t>['Education', 'Engineering', 'Campus', 'Placement', 'Skills', 'Machine Learning', 'Software', 'Web Development', 'Profile Building']</t>
-        </is>
-      </c>
-      <c r="E77" t="n">
+      <c r="D77" t="n">
         <v>2562</v>
       </c>
+      <c r="E77" t="inlineStr">
+        <is>
+          <t>2021-06-24T14:30:16Z</t>
+        </is>
+      </c>
       <c r="F77" t="inlineStr">
         <is>
-          <t>2021-06-24T14:30:16Z</t>
+          <t>1478</t>
         </is>
       </c>
       <c r="G77" t="inlineStr">
         <is>
-          <t>1477</t>
-        </is>
-      </c>
-      <c r="H77" t="inlineStr">
-        <is>
-          <t>50383</t>
+          <t>50425</t>
         </is>
       </c>
     </row>
@@ -3368,27 +2987,22 @@
           <t>Softmax Regression || Multinomial Logistic Regression || Logistic Regression Part 6</t>
         </is>
       </c>
-      <c r="D78" t="inlineStr">
-        <is>
-          <t>['Education', 'Engineering', 'Campus', 'Placement', 'Skills', 'Machine Learning', 'Software', 'Web Development', 'Profile Building']</t>
-        </is>
-      </c>
-      <c r="E78" t="n">
+      <c r="D78" t="n">
         <v>2301</v>
       </c>
+      <c r="E78" t="inlineStr">
+        <is>
+          <t>2021-06-28T14:30:03Z</t>
+        </is>
+      </c>
       <c r="F78" t="inlineStr">
         <is>
-          <t>2021-06-28T14:30:03Z</t>
+          <t>1041</t>
         </is>
       </c>
       <c r="G78" t="inlineStr">
         <is>
-          <t>1039</t>
-        </is>
-      </c>
-      <c r="H78" t="inlineStr">
-        <is>
-          <t>39856</t>
+          <t>39884</t>
         </is>
       </c>
     </row>
@@ -3406,27 +3020,22 @@
           <t>Polynomial Features in Logistic Regression | Non Linear Logistic Regression | Logistic Regression 7</t>
         </is>
       </c>
-      <c r="D79" t="inlineStr">
-        <is>
-          <t>['Education', 'Engineering', 'Campus', 'Placement', 'Skills', 'Machine Learning', 'Software', 'Web Development', 'Profile Building']</t>
-        </is>
-      </c>
-      <c r="E79" t="n">
+      <c r="D79" t="n">
         <v>551</v>
       </c>
+      <c r="E79" t="inlineStr">
+        <is>
+          <t>2021-06-29T14:30:05Z</t>
+        </is>
+      </c>
       <c r="F79" t="inlineStr">
         <is>
-          <t>2021-06-29T14:30:05Z</t>
+          <t>649</t>
         </is>
       </c>
       <c r="G79" t="inlineStr">
         <is>
-          <t>648</t>
-        </is>
-      </c>
-      <c r="H79" t="inlineStr">
-        <is>
-          <t>20317</t>
+          <t>20333</t>
         </is>
       </c>
     </row>
@@ -3444,27 +3053,22 @@
           <t>Logistic Regression Hyperparameters || Logistic Regression Part 8</t>
         </is>
       </c>
-      <c r="D80" t="inlineStr">
-        <is>
-          <t>['Education', 'Engineering', 'Campus', 'Placement', 'Skills', 'Machine Learning', 'Software', 'Web Development', 'Profile Building']</t>
-        </is>
-      </c>
-      <c r="E80" t="n">
+      <c r="D80" t="n">
         <v>787</v>
       </c>
+      <c r="E80" t="inlineStr">
+        <is>
+          <t>2021-06-30T14:30:00Z</t>
+        </is>
+      </c>
       <c r="F80" t="inlineStr">
         <is>
-          <t>2021-06-30T14:30:00Z</t>
+          <t>655</t>
         </is>
       </c>
       <c r="G80" t="inlineStr">
         <is>
-          <t>654</t>
-        </is>
-      </c>
-      <c r="H80" t="inlineStr">
-        <is>
-          <t>27417</t>
+          <t>27428</t>
         </is>
       </c>
     </row>
@@ -3482,27 +3086,22 @@
           <t>Decision Trees Geometric Intuition | Entropy | Gini impurity | Information Gain</t>
         </is>
       </c>
-      <c r="D81" t="inlineStr">
-        <is>
-          <t>['Education', 'Engineering', 'Campus', 'Placement', 'Skills', 'Machine Learning', 'Software', 'Web Development', 'Profile Building']</t>
-        </is>
-      </c>
-      <c r="E81" t="n">
+      <c r="D81" t="n">
         <v>3509</v>
       </c>
+      <c r="E81" t="inlineStr">
+        <is>
+          <t>2021-07-02T14:30:01Z</t>
+        </is>
+      </c>
       <c r="F81" t="inlineStr">
         <is>
-          <t>2021-07-02T14:30:01Z</t>
+          <t>2012</t>
         </is>
       </c>
       <c r="G81" t="inlineStr">
         <is>
-          <t>2010</t>
-        </is>
-      </c>
-      <c r="H81" t="inlineStr">
-        <is>
-          <t>93874</t>
+          <t>93917</t>
         </is>
       </c>
     </row>
@@ -3520,27 +3119,22 @@
           <t>Decision Trees - Hyperparameters | Overfitting and Underfitting in Decision Trees</t>
         </is>
       </c>
-      <c r="D82" t="inlineStr">
-        <is>
-          <t>['Education', 'Engineering', 'Campus', 'Placement', 'Skills', 'Machine Learning', 'Software', 'Web Development', 'Profile Building']</t>
-        </is>
-      </c>
-      <c r="E82" t="n">
+      <c r="D82" t="n">
         <v>1643</v>
       </c>
+      <c r="E82" t="inlineStr">
+        <is>
+          <t>2021-07-03T14:30:06Z</t>
+        </is>
+      </c>
       <c r="F82" t="inlineStr">
         <is>
-          <t>2021-07-03T14:30:06Z</t>
+          <t>1733</t>
         </is>
       </c>
       <c r="G82" t="inlineStr">
         <is>
-          <t>1731</t>
-        </is>
-      </c>
-      <c r="H82" t="inlineStr">
-        <is>
-          <t>45012</t>
+          <t>45047</t>
         </is>
       </c>
     </row>
@@ -3558,27 +3152,22 @@
           <t>Regression Trees | Decision Trees Part 3</t>
         </is>
       </c>
-      <c r="D83" t="inlineStr">
-        <is>
-          <t>['Education', 'Engineering', 'Campus', 'Placement', 'Skills', 'Machine Learning', 'Software', 'Web Development', 'Profile Building']</t>
-        </is>
-      </c>
-      <c r="E83" t="n">
+      <c r="D83" t="n">
         <v>2115</v>
       </c>
+      <c r="E83" t="inlineStr">
+        <is>
+          <t>2021-07-05T14:30:09Z</t>
+        </is>
+      </c>
       <c r="F83" t="inlineStr">
         <is>
-          <t>2021-07-05T14:30:09Z</t>
+          <t>858</t>
         </is>
       </c>
       <c r="G83" t="inlineStr">
         <is>
-          <t>858</t>
-        </is>
-      </c>
-      <c r="H83" t="inlineStr">
-        <is>
-          <t>32212</t>
+          <t>32219</t>
         </is>
       </c>
     </row>
@@ -3596,27 +3185,22 @@
           <t>Awesome Decision Tree Visualization using dtreeviz library</t>
         </is>
       </c>
-      <c r="D84" t="inlineStr">
-        <is>
-          <t>['Decision trees', 'Machine learning', 'Visualization']</t>
-        </is>
-      </c>
-      <c r="E84" t="n">
+      <c r="D84" t="n">
         <v>1116</v>
       </c>
+      <c r="E84" t="inlineStr">
+        <is>
+          <t>2021-03-19T13:49:09Z</t>
+        </is>
+      </c>
       <c r="F84" t="inlineStr">
         <is>
-          <t>2021-03-19T13:49:09Z</t>
+          <t>789</t>
         </is>
       </c>
       <c r="G84" t="inlineStr">
         <is>
-          <t>789</t>
-        </is>
-      </c>
-      <c r="H84" t="inlineStr">
-        <is>
-          <t>25122</t>
+          <t>25141</t>
         </is>
       </c>
     </row>
@@ -3634,27 +3218,22 @@
           <t>Introduction to Ensemble Learning | Ensemble Techniques in Machine Learning</t>
         </is>
       </c>
-      <c r="D85" t="inlineStr">
-        <is>
-          <t>['Education', 'Engineering', 'Campus', 'Placement', 'Skills', 'Machine Learning', 'Software', 'Web Development', 'Profile Building']</t>
-        </is>
-      </c>
-      <c r="E85" t="n">
+      <c r="D85" t="n">
         <v>2263</v>
       </c>
+      <c r="E85" t="inlineStr">
+        <is>
+          <t>2021-07-12T14:30:15Z</t>
+        </is>
+      </c>
       <c r="F85" t="inlineStr">
         <is>
-          <t>2021-07-12T14:30:15Z</t>
+          <t>2096</t>
         </is>
       </c>
       <c r="G85" t="inlineStr">
         <is>
-          <t>2093</t>
-        </is>
-      </c>
-      <c r="H85" t="inlineStr">
-        <is>
-          <t>75592</t>
+          <t>75639</t>
         </is>
       </c>
     </row>
@@ -3672,27 +3251,22 @@
           <t>Voting Ensemble |  Introduction and Core Idea | Part 1</t>
         </is>
       </c>
-      <c r="D86" t="inlineStr">
-        <is>
-          <t>['Ensemble Learning', 'Machine Learning']</t>
-        </is>
-      </c>
-      <c r="E86" t="n">
+      <c r="D86" t="n">
         <v>990</v>
       </c>
+      <c r="E86" t="inlineStr">
+        <is>
+          <t>2021-03-09T13:17:07Z</t>
+        </is>
+      </c>
       <c r="F86" t="inlineStr">
         <is>
-          <t>2021-03-09T13:17:07Z</t>
+          <t>921</t>
         </is>
       </c>
       <c r="G86" t="inlineStr">
         <is>
-          <t>920</t>
-        </is>
-      </c>
-      <c r="H86" t="inlineStr">
-        <is>
-          <t>27498</t>
+          <t>27522</t>
         </is>
       </c>
     </row>
@@ -3710,27 +3284,22 @@
           <t>Voting Ensemble | Classification | Voting Classifier | Hard Voting Vs Soft Voting | Part 2</t>
         </is>
       </c>
-      <c r="D87" t="inlineStr">
-        <is>
-          <t>['Machine Learning', 'Ensemble Learning', 'Voting Classifier']</t>
-        </is>
-      </c>
-      <c r="E87" t="n">
+      <c r="D87" t="n">
         <v>1430</v>
       </c>
+      <c r="E87" t="inlineStr">
+        <is>
+          <t>2021-03-10T14:13:57Z</t>
+        </is>
+      </c>
       <c r="F87" t="inlineStr">
         <is>
-          <t>2021-03-10T14:13:57Z</t>
+          <t>886</t>
         </is>
       </c>
       <c r="G87" t="inlineStr">
         <is>
-          <t>885</t>
-        </is>
-      </c>
-      <c r="H87" t="inlineStr">
-        <is>
-          <t>25662</t>
+          <t>25695</t>
         </is>
       </c>
     </row>
@@ -3748,27 +3317,22 @@
           <t>Voting Ensemble | Regression | Part 3</t>
         </is>
       </c>
-      <c r="D88" t="inlineStr">
-        <is>
-          <t>['Machine Learning', 'Ensemble Learning']</t>
-        </is>
-      </c>
-      <c r="E88" t="n">
+      <c r="D88" t="n">
         <v>657</v>
       </c>
+      <c r="E88" t="inlineStr">
+        <is>
+          <t>2021-03-11T14:06:31Z</t>
+        </is>
+      </c>
       <c r="F88" t="inlineStr">
         <is>
-          <t>2021-03-11T14:06:31Z</t>
+          <t>683</t>
         </is>
       </c>
       <c r="G88" t="inlineStr">
         <is>
-          <t>683</t>
-        </is>
-      </c>
-      <c r="H88" t="inlineStr">
-        <is>
-          <t>17695</t>
+          <t>17723</t>
         </is>
       </c>
     </row>
@@ -3786,23 +3350,22 @@
           <t>Bagging | Introduction | Part 1</t>
         </is>
       </c>
-      <c r="D89" t="inlineStr"/>
-      <c r="E89" t="n">
+      <c r="D89" t="n">
         <v>1873</v>
       </c>
+      <c r="E89" t="inlineStr">
+        <is>
+          <t>2021-03-12T15:25:14Z</t>
+        </is>
+      </c>
       <c r="F89" t="inlineStr">
         <is>
-          <t>2021-03-12T15:25:14Z</t>
+          <t>1235</t>
         </is>
       </c>
       <c r="G89" t="inlineStr">
         <is>
-          <t>1234</t>
-        </is>
-      </c>
-      <c r="H89" t="inlineStr">
-        <is>
-          <t>45505</t>
+          <t>45550</t>
         </is>
       </c>
     </row>
@@ -3820,23 +3383,22 @@
           <t>Bagging Ensemble | Part 2 | Bagging Classifiers</t>
         </is>
       </c>
-      <c r="D90" t="inlineStr"/>
-      <c r="E90" t="n">
+      <c r="D90" t="n">
         <v>1352</v>
       </c>
+      <c r="E90" t="inlineStr">
+        <is>
+          <t>2021-03-16T13:37:35Z</t>
+        </is>
+      </c>
       <c r="F90" t="inlineStr">
         <is>
-          <t>2021-03-16T13:37:35Z</t>
+          <t>932</t>
         </is>
       </c>
       <c r="G90" t="inlineStr">
         <is>
-          <t>931</t>
-        </is>
-      </c>
-      <c r="H90" t="inlineStr">
-        <is>
-          <t>26688</t>
+          <t>26720</t>
         </is>
       </c>
     </row>
@@ -3854,23 +3416,22 @@
           <t>Bagging Ensemble | Part 3 | Bagging Regressor</t>
         </is>
       </c>
-      <c r="D91" t="inlineStr"/>
-      <c r="E91" t="n">
+      <c r="D91" t="n">
         <v>655</v>
       </c>
+      <c r="E91" t="inlineStr">
+        <is>
+          <t>2021-03-17T19:49:37Z</t>
+        </is>
+      </c>
       <c r="F91" t="inlineStr">
         <is>
-          <t>2021-03-17T19:49:37Z</t>
+          <t>802</t>
         </is>
       </c>
       <c r="G91" t="inlineStr">
         <is>
-          <t>800</t>
-        </is>
-      </c>
-      <c r="H91" t="inlineStr">
-        <is>
-          <t>19371</t>
+          <t>19391</t>
         </is>
       </c>
     </row>
@@ -3888,27 +3449,22 @@
           <t>Introduction to Random Forest | Intuition behind the Algorithm</t>
         </is>
       </c>
-      <c r="D92" t="inlineStr">
-        <is>
-          <t>['Education', 'Engineering', 'Campus', 'Placement', 'Skills', 'Machine Learning', 'Software', 'Web Development', 'Profile Building']</t>
-        </is>
-      </c>
-      <c r="E92" t="n">
+      <c r="D92" t="n">
         <v>2035</v>
       </c>
+      <c r="E92" t="inlineStr">
+        <is>
+          <t>2021-07-19T15:13:28Z</t>
+        </is>
+      </c>
       <c r="F92" t="inlineStr">
         <is>
-          <t>2021-07-19T15:13:28Z</t>
+          <t>1322</t>
         </is>
       </c>
       <c r="G92" t="inlineStr">
         <is>
-          <t>1321</t>
-        </is>
-      </c>
-      <c r="H92" t="inlineStr">
-        <is>
-          <t>54114</t>
+          <t>54143</t>
         </is>
       </c>
     </row>
@@ -3926,27 +3482,22 @@
           <t>How Random Forest Performs So Well? Bias Variance Trade-Off in Random Forest</t>
         </is>
       </c>
-      <c r="D93" t="inlineStr">
-        <is>
-          <t>['Education', 'Engineering', 'Campus', 'Placement', 'Skills', 'Machine Learning', 'Software', 'Web Development', 'Profile Building']</t>
-        </is>
-      </c>
-      <c r="E93" t="n">
+      <c r="D93" t="n">
         <v>772</v>
       </c>
+      <c r="E93" t="inlineStr">
+        <is>
+          <t>2021-07-20T14:30:08Z</t>
+        </is>
+      </c>
       <c r="F93" t="inlineStr">
         <is>
-          <t>2021-07-20T14:30:08Z</t>
+          <t>749</t>
         </is>
       </c>
       <c r="G93" t="inlineStr">
         <is>
-          <t>748</t>
-        </is>
-      </c>
-      <c r="H93" t="inlineStr">
-        <is>
-          <t>27485</t>
+          <t>27511</t>
         </is>
       </c>
     </row>
@@ -3964,27 +3515,22 @@
           <t>Bagging Vs Random Forest | What is the difference between Bagging and Random Forest | Very Important</t>
         </is>
       </c>
-      <c r="D94" t="inlineStr">
-        <is>
-          <t>['Education', 'Engineering', 'Campus', 'Placement', 'Skills', 'Machine Learning', 'Software', 'Web Development', 'Profile Building']</t>
-        </is>
-      </c>
-      <c r="E94" t="n">
+      <c r="D94" t="n">
         <v>722</v>
       </c>
+      <c r="E94" t="inlineStr">
+        <is>
+          <t>2021-07-22T14:30:06Z</t>
+        </is>
+      </c>
       <c r="F94" t="inlineStr">
         <is>
-          <t>2021-07-22T14:30:06Z</t>
+          <t>879</t>
         </is>
       </c>
       <c r="G94" t="inlineStr">
         <is>
-          <t>878</t>
-        </is>
-      </c>
-      <c r="H94" t="inlineStr">
-        <is>
-          <t>27242</t>
+          <t>27265</t>
         </is>
       </c>
     </row>
@@ -4002,27 +3548,22 @@
           <t>Random Forest Hyper-parameters</t>
         </is>
       </c>
-      <c r="D95" t="inlineStr">
-        <is>
-          <t>['Education', 'Engineering', 'Campus', 'Placement', 'Skills', 'Machine Learning', 'Software', 'Web Development', 'Profile Building']</t>
-        </is>
-      </c>
-      <c r="E95" t="n">
+      <c r="D95" t="n">
         <v>917</v>
       </c>
+      <c r="E95" t="inlineStr">
+        <is>
+          <t>2021-07-23T14:30:05Z</t>
+        </is>
+      </c>
       <c r="F95" t="inlineStr">
         <is>
-          <t>2021-07-23T14:30:05Z</t>
+          <t>811</t>
         </is>
       </c>
       <c r="G95" t="inlineStr">
         <is>
-          <t>809</t>
-        </is>
-      </c>
-      <c r="H95" t="inlineStr">
-        <is>
-          <t>30837</t>
+          <t>30866</t>
         </is>
       </c>
     </row>
@@ -4040,27 +3581,22 @@
           <t>Hyperparameter Tuning Random Forest using GridSearchCV and RandomizedSearchCV | Code Example</t>
         </is>
       </c>
-      <c r="D96" t="inlineStr">
-        <is>
-          <t>['Education', 'Engineering', 'Campus', 'Placement', 'Skills', 'Machine Learning', 'Software', 'Web Development', 'Profile Building']</t>
-        </is>
-      </c>
-      <c r="E96" t="n">
+      <c r="D96" t="n">
         <v>704</v>
       </c>
+      <c r="E96" t="inlineStr">
+        <is>
+          <t>2021-07-26T14:30:01Z</t>
+        </is>
+      </c>
       <c r="F96" t="inlineStr">
         <is>
-          <t>2021-07-26T14:30:01Z</t>
+          <t>924</t>
         </is>
       </c>
       <c r="G96" t="inlineStr">
         <is>
-          <t>923</t>
-        </is>
-      </c>
-      <c r="H96" t="inlineStr">
-        <is>
-          <t>37459</t>
+          <t>37475</t>
         </is>
       </c>
     </row>
@@ -4078,27 +3614,22 @@
           <t>OOB Score | Out of Bag Evaluation in Random Forest | Machine Learning</t>
         </is>
       </c>
-      <c r="D97" t="inlineStr">
-        <is>
-          <t>['Machine Learning', 'machine learning', 'random forest', 'python', 'out of bag error', 'random forest intro', 'random forest machine learning']</t>
-        </is>
-      </c>
-      <c r="E97" t="n">
+      <c r="D97" t="n">
         <v>405</v>
       </c>
+      <c r="E97" t="inlineStr">
+        <is>
+          <t>2021-07-28T14:30:08Z</t>
+        </is>
+      </c>
       <c r="F97" t="inlineStr">
         <is>
-          <t>2021-07-28T14:30:08Z</t>
+          <t>621</t>
         </is>
       </c>
       <c r="G97" t="inlineStr">
         <is>
-          <t>620</t>
-        </is>
-      </c>
-      <c r="H97" t="inlineStr">
-        <is>
-          <t>21056</t>
+          <t>21068</t>
         </is>
       </c>
     </row>
@@ -4116,27 +3647,22 @@
           <t>Feature Importance using Random Forest and Decision Trees | How is Feature Importance calculated</t>
         </is>
       </c>
-      <c r="D98" t="inlineStr">
-        <is>
-          <t>['machine learning', 'machine learning course', 'machine learning algorithms', 'machine learning explained', 'machine learning algorithms for data science', 'feature importance', 'feature importance in decision trees', 'feature importance in random forest', 'random forest', 'sklearn random forest', 'end to end machine learning', 'feature selection', 'random forest algorithm', 'random forest regression']</t>
-        </is>
-      </c>
-      <c r="E98" t="n">
+      <c r="D98" t="n">
         <v>1640</v>
       </c>
+      <c r="E98" t="inlineStr">
+        <is>
+          <t>2021-07-30T14:30:04Z</t>
+        </is>
+      </c>
       <c r="F98" t="inlineStr">
         <is>
-          <t>2021-07-30T14:30:04Z</t>
+          <t>985</t>
         </is>
       </c>
       <c r="G98" t="inlineStr">
         <is>
-          <t>983</t>
-        </is>
-      </c>
-      <c r="H98" t="inlineStr">
-        <is>
-          <t>35751</t>
+          <t>35772</t>
         </is>
       </c>
     </row>
@@ -4154,23 +3680,22 @@
           <t>How Adaboost Classifier Works? | Geometric Intuition</t>
         </is>
       </c>
-      <c r="D99" t="inlineStr"/>
-      <c r="E99" t="n">
+      <c r="D99" t="n">
         <v>1034</v>
       </c>
+      <c r="E99" t="inlineStr">
+        <is>
+          <t>2021-08-09T14:30:15Z</t>
+        </is>
+      </c>
       <c r="F99" t="inlineStr">
         <is>
-          <t>2021-08-09T14:30:15Z</t>
+          <t>1035</t>
         </is>
       </c>
       <c r="G99" t="inlineStr">
         <is>
-          <t>1033</t>
-        </is>
-      </c>
-      <c r="H99" t="inlineStr">
-        <is>
-          <t>38930</t>
+          <t>38964</t>
         </is>
       </c>
     </row>
@@ -4188,23 +3713,22 @@
           <t>AdaBoost - A Step by Step Explanation</t>
         </is>
       </c>
-      <c r="D100" t="inlineStr"/>
-      <c r="E100" t="n">
+      <c r="D100" t="n">
         <v>1163</v>
       </c>
+      <c r="E100" t="inlineStr">
+        <is>
+          <t>2021-08-10T14:30:10Z</t>
+        </is>
+      </c>
       <c r="F100" t="inlineStr">
         <is>
-          <t>2021-08-10T14:30:10Z</t>
+          <t>1240</t>
         </is>
       </c>
       <c r="G100" t="inlineStr">
         <is>
-          <t>1239</t>
-        </is>
-      </c>
-      <c r="H100" t="inlineStr">
-        <is>
-          <t>40544</t>
+          <t>40584</t>
         </is>
       </c>
     </row>
@@ -4222,27 +3746,22 @@
           <t>AdaBoost Algorithm | Code from Scratch</t>
         </is>
       </c>
-      <c r="D101" t="inlineStr">
-        <is>
-          <t>['Education', 'Engineering', 'Campus', 'Placement', 'Skills', 'Machine Learning', 'Software', 'Web Development', 'Profile Building']</t>
-        </is>
-      </c>
-      <c r="E101" t="n">
+      <c r="D101" t="n">
         <v>987</v>
       </c>
+      <c r="E101" t="inlineStr">
+        <is>
+          <t>2021-08-16T14:30:00Z</t>
+        </is>
+      </c>
       <c r="F101" t="inlineStr">
         <is>
-          <t>2021-08-16T14:30:00Z</t>
+          <t>686</t>
         </is>
       </c>
       <c r="G101" t="inlineStr">
         <is>
-          <t>686</t>
-        </is>
-      </c>
-      <c r="H101" t="inlineStr">
-        <is>
-          <t>25349</t>
+          <t>25373</t>
         </is>
       </c>
     </row>
@@ -4260,27 +3779,22 @@
           <t>AdaBoost Hyperparameters | GridSearchCV in Adaboost</t>
         </is>
       </c>
-      <c r="D102" t="inlineStr">
-        <is>
-          <t>['Machine Learning', 'adaboost algorithm', 'adaboost algorithm in machine learning', 'adaptive boosting machine learning', 'boosting machine learning', 'adaptive boosting']</t>
-        </is>
-      </c>
-      <c r="E102" t="n">
+      <c r="D102" t="n">
         <v>673</v>
       </c>
+      <c r="E102" t="inlineStr">
+        <is>
+          <t>2021-08-17T14:30:02Z</t>
+        </is>
+      </c>
       <c r="F102" t="inlineStr">
         <is>
-          <t>2021-08-17T14:30:02Z</t>
+          <t>527</t>
         </is>
       </c>
       <c r="G102" t="inlineStr">
         <is>
-          <t>527</t>
-        </is>
-      </c>
-      <c r="H102" t="inlineStr">
-        <is>
-          <t>18620</t>
+          <t>18633</t>
         </is>
       </c>
     </row>
@@ -4298,23 +3812,22 @@
           <t>Bagging Vs Boosting | What is the difference between Bagging and Boosting</t>
         </is>
       </c>
-      <c r="D103" t="inlineStr"/>
-      <c r="E103" t="n">
+      <c r="D103" t="n">
         <v>377</v>
       </c>
+      <c r="E103" t="inlineStr">
+        <is>
+          <t>2021-08-18T14:30:01Z</t>
+        </is>
+      </c>
       <c r="F103" t="inlineStr">
         <is>
-          <t>2021-08-18T14:30:01Z</t>
+          <t>1018</t>
         </is>
       </c>
       <c r="G103" t="inlineStr">
         <is>
-          <t>1017</t>
-        </is>
-      </c>
-      <c r="H103" t="inlineStr">
-        <is>
-          <t>33251</t>
+          <t>33270</t>
         </is>
       </c>
     </row>
@@ -4332,27 +3845,22 @@
           <t>K-Means Clustering Algorithm | Geometric Intuition | Clustering | Unsupervised Learning</t>
         </is>
       </c>
-      <c r="D104" t="inlineStr">
-        <is>
-          <t>['k means clustering', 'k means clustering algorithm', 'k means', 'clustering algorithms', 'clustering algorithms python', 'clustering algorithms machine learning', 'unsupervised machine learning', 'elbow method', 'elbow curve kmeans', 'campusx', 'machine learning algorithms for data science']</t>
-        </is>
-      </c>
-      <c r="E104" t="n">
+      <c r="D104" t="n">
         <v>1438</v>
       </c>
+      <c r="E104" t="inlineStr">
+        <is>
+          <t>2021-08-24T14:30:01Z</t>
+        </is>
+      </c>
       <c r="F104" t="inlineStr">
         <is>
-          <t>2021-08-24T14:30:01Z</t>
+          <t>2434</t>
         </is>
       </c>
       <c r="G104" t="inlineStr">
         <is>
-          <t>2433</t>
-        </is>
-      </c>
-      <c r="H104" t="inlineStr">
-        <is>
-          <t>84561</t>
+          <t>84638</t>
         </is>
       </c>
     </row>
@@ -4370,27 +3878,22 @@
           <t>K-Means Clustering Algorithm in Python | Practical Example | Student Clustering Example | sklearn</t>
         </is>
       </c>
-      <c r="D105" t="inlineStr">
-        <is>
-          <t>['k means in hindi', 'k means kya hota hai', 'k means clustering algorithm', 'k means clustering', 'kmeans in python', 'kmeans practical example', 'kmeans sklearn', 'unsupervised learning', 'campusx', 'Nitish Singh Campusx', 'machine learning algorithms for data science', 'customer clustering', 'customer segmentation']</t>
-        </is>
-      </c>
-      <c r="E105" t="n">
+      <c r="D105" t="n">
         <v>613</v>
       </c>
+      <c r="E105" t="inlineStr">
+        <is>
+          <t>2021-08-26T14:30:11Z</t>
+        </is>
+      </c>
       <c r="F105" t="inlineStr">
         <is>
-          <t>2021-08-26T14:30:11Z</t>
+          <t>1459</t>
         </is>
       </c>
       <c r="G105" t="inlineStr">
         <is>
-          <t>1459</t>
-        </is>
-      </c>
-      <c r="H105" t="inlineStr">
-        <is>
-          <t>53001</t>
+          <t>53017</t>
         </is>
       </c>
     </row>
@@ -4408,27 +3911,22 @@
           <t>K-Means Clustering Algorithm From Scratch In Python | ML Algorithms From Scratch</t>
         </is>
       </c>
-      <c r="D106" t="inlineStr">
-        <is>
-          <t>['k means clustering algorithm', 'kmeans clustering algorithm from scratch', 'kmeans from scratch in python', 'ml algorithms from scratch in python', 'unsupervised learning', 'campusx', 'Nitish Singh Campusx']</t>
-        </is>
-      </c>
-      <c r="E106" t="n">
+      <c r="D106" t="n">
         <v>2033</v>
       </c>
+      <c r="E106" t="inlineStr">
+        <is>
+          <t>2021-08-25T14:30:02Z</t>
+        </is>
+      </c>
       <c r="F106" t="inlineStr">
         <is>
-          <t>2021-08-25T14:30:02Z</t>
+          <t>1032</t>
         </is>
       </c>
       <c r="G106" t="inlineStr">
         <is>
-          <t>1032</t>
-        </is>
-      </c>
-      <c r="H106" t="inlineStr">
-        <is>
-          <t>37741</t>
+          <t>37758</t>
         </is>
       </c>
     </row>
@@ -4446,27 +3944,22 @@
           <t>Gradient Boosting Explained | How Gradient Boosting Works?</t>
         </is>
       </c>
-      <c r="D107" t="inlineStr">
-        <is>
-          <t>['Gradient Boosting', 'Boosting', 'Ensemble Learning', 'Machine Learning Algorithms', 'Machine Learning Course', 'Campusx', 'Nitish Singh CampusX']</t>
-        </is>
-      </c>
-      <c r="E107" t="n">
+      <c r="D107" t="n">
         <v>1969</v>
       </c>
+      <c r="E107" t="inlineStr">
+        <is>
+          <t>2021-09-09T13:30:13Z</t>
+        </is>
+      </c>
       <c r="F107" t="inlineStr">
         <is>
-          <t>2021-09-09T13:30:13Z</t>
+          <t>1846</t>
         </is>
       </c>
       <c r="G107" t="inlineStr">
         <is>
-          <t>1845</t>
-        </is>
-      </c>
-      <c r="H107" t="inlineStr">
-        <is>
-          <t>61884</t>
+          <t>61921</t>
         </is>
       </c>
     </row>
@@ -4484,27 +3977,22 @@
           <t>Gradient Boosting Regression Part 2 | Mathematics of Gradient Boosting</t>
         </is>
       </c>
-      <c r="D108" t="inlineStr">
-        <is>
-          <t>['campusx', 'gradient boosting', 'gradient boosting regression', 'gradient boost maths', 'boosting techniques', 'machine learning algorithms', 'nitish sir campusx', 'nitish singh campusx', '100 days of machine learning', 'machine learning course']</t>
-        </is>
-      </c>
-      <c r="E108" t="n">
+      <c r="D108" t="n">
         <v>3402</v>
       </c>
+      <c r="E108" t="inlineStr">
+        <is>
+          <t>2021-09-20T13:30:19Z</t>
+        </is>
+      </c>
       <c r="F108" t="inlineStr">
         <is>
-          <t>2021-09-20T13:30:19Z</t>
+          <t>907</t>
         </is>
       </c>
       <c r="G108" t="inlineStr">
         <is>
-          <t>907</t>
-        </is>
-      </c>
-      <c r="H108" t="inlineStr">
-        <is>
-          <t>30403</t>
+          <t>30418</t>
         </is>
       </c>
     </row>
@@ -4522,27 +4010,22 @@
           <t>Gradient Boosting for Classification | Geometric Intuition | CampusX</t>
         </is>
       </c>
-      <c r="D109" t="inlineStr">
-        <is>
-          <t>['Education', 'Engineering', 'Campus', 'Placement', 'Skills', 'Machine Learning', 'Software', 'Web Development', 'Profile Building']</t>
-        </is>
-      </c>
-      <c r="E109" t="n">
+      <c r="D109" t="n">
         <v>3873</v>
       </c>
+      <c r="E109" t="inlineStr">
+        <is>
+          <t>2023-08-08T14:00:04Z</t>
+        </is>
+      </c>
       <c r="F109" t="inlineStr">
         <is>
-          <t>2023-08-08T14:00:04Z</t>
+          <t>805</t>
         </is>
       </c>
       <c r="G109" t="inlineStr">
         <is>
-          <t>805</t>
-        </is>
-      </c>
-      <c r="H109" t="inlineStr">
-        <is>
-          <t>25989</t>
+          <t>25999</t>
         </is>
       </c>
     </row>
@@ -4560,23 +4043,22 @@
           <t>Stacking and Blending Ensembles</t>
         </is>
       </c>
-      <c r="D110" t="inlineStr"/>
-      <c r="E110" t="n">
+      <c r="D110" t="n">
         <v>2120</v>
       </c>
+      <c r="E110" t="inlineStr">
+        <is>
+          <t>2021-09-30T13:30:09Z</t>
+        </is>
+      </c>
       <c r="F110" t="inlineStr">
         <is>
-          <t>2021-09-30T13:30:09Z</t>
+          <t>822</t>
         </is>
       </c>
       <c r="G110" t="inlineStr">
         <is>
-          <t>822</t>
-        </is>
-      </c>
-      <c r="H110" t="inlineStr">
-        <is>
-          <t>22802</t>
+          <t>22812</t>
         </is>
       </c>
     </row>
@@ -4594,27 +4076,22 @@
           <t>Agglomerative Hierarchical Clustering | Python Code Example</t>
         </is>
       </c>
-      <c r="D111" t="inlineStr">
-        <is>
-          <t>['Education', 'Engineering', 'Campus', 'Placement', 'Skills', 'Machine Learning', 'Software', 'Web Development', 'Profile Building']</t>
-        </is>
-      </c>
-      <c r="E111" t="n">
+      <c r="D111" t="n">
         <v>2243</v>
       </c>
+      <c r="E111" t="inlineStr">
+        <is>
+          <t>2021-11-07T14:00:06Z</t>
+        </is>
+      </c>
       <c r="F111" t="inlineStr">
         <is>
-          <t>2021-11-07T14:00:06Z</t>
+          <t>1243</t>
         </is>
       </c>
       <c r="G111" t="inlineStr">
         <is>
-          <t>1243</t>
-        </is>
-      </c>
-      <c r="H111" t="inlineStr">
-        <is>
-          <t>38073</t>
+          <t>38089</t>
         </is>
       </c>
     </row>
@@ -4632,27 +4109,22 @@
           <t>What is K Nearest Neighbors? | KNN Explained in Hindi | Simple Overview in 1 Video | CampusX</t>
         </is>
       </c>
-      <c r="D112" t="inlineStr">
-        <is>
-          <t>['Education', 'Engineering', 'Campus', 'Placement', 'Skills', 'Machine Learning', 'Software', 'Web Development', 'Profile Building']</t>
-        </is>
-      </c>
-      <c r="E112" t="n">
+      <c r="D112" t="n">
         <v>3121</v>
       </c>
+      <c r="E112" t="inlineStr">
+        <is>
+          <t>2023-05-23T16:00:11Z</t>
+        </is>
+      </c>
       <c r="F112" t="inlineStr">
         <is>
-          <t>2023-05-23T16:00:11Z</t>
+          <t>1387</t>
         </is>
       </c>
       <c r="G112" t="inlineStr">
         <is>
-          <t>1386</t>
-        </is>
-      </c>
-      <c r="H112" t="inlineStr">
-        <is>
-          <t>49934</t>
+          <t>49968</t>
         </is>
       </c>
     </row>
@@ -4670,27 +4142,22 @@
           <t>What are the main Assumptions of Linear Regression? | Top 5 Assumptions of Linear Regression</t>
         </is>
       </c>
-      <c r="D113" t="inlineStr">
-        <is>
-          <t>['assumptions of linear regression', 'what are the assumptions for a linear regression model', 'linear regression assumptions machine learning', 'linear regression assumptions explained', 'linear regression assumptions python', 'linear regression assumptions linearity', 'multiple linear regression assumptions', 'campusx', 'how to check linear regression assumptions', 'checking assumptions of linear regression in python', 'python code to check linear regression assumption']</t>
-        </is>
-      </c>
-      <c r="E113" t="n">
+      <c r="D113" t="n">
         <v>1058</v>
       </c>
+      <c r="E113" t="inlineStr">
+        <is>
+          <t>2022-06-20T14:00:07Z</t>
+        </is>
+      </c>
       <c r="F113" t="inlineStr">
         <is>
-          <t>2022-06-20T14:00:07Z</t>
+          <t>2039</t>
         </is>
       </c>
       <c r="G113" t="inlineStr">
         <is>
-          <t>2036</t>
-        </is>
-      </c>
-      <c r="H113" t="inlineStr">
-        <is>
-          <t>46527</t>
+          <t>46567</t>
         </is>
       </c>
     </row>
@@ -4708,23 +4175,22 @@
           <t>Support Vector Machines | Geometric Intuition</t>
         </is>
       </c>
-      <c r="D114" t="inlineStr"/>
-      <c r="E114" t="n">
+      <c r="D114" t="n">
         <v>706</v>
       </c>
+      <c r="E114" t="inlineStr">
+        <is>
+          <t>2020-07-10T01:54:27Z</t>
+        </is>
+      </c>
       <c r="F114" t="inlineStr">
         <is>
-          <t>2020-07-10T01:54:27Z</t>
+          <t>1815</t>
         </is>
       </c>
       <c r="G114" t="inlineStr">
         <is>
-          <t>1813</t>
-        </is>
-      </c>
-      <c r="H114" t="inlineStr">
-        <is>
-          <t>98510</t>
+          <t>98578</t>
         </is>
       </c>
     </row>
@@ -4742,27 +4208,22 @@
           <t>Mathematics of SVM | Support Vector Machines | Hard margin SVM</t>
         </is>
       </c>
-      <c r="D115" t="inlineStr">
-        <is>
-          <t>['InShot']</t>
-        </is>
-      </c>
-      <c r="E115" t="n">
+      <c r="D115" t="n">
         <v>2094</v>
       </c>
+      <c r="E115" t="inlineStr">
+        <is>
+          <t>2020-07-10T01:55:41Z</t>
+        </is>
+      </c>
       <c r="F115" t="inlineStr">
         <is>
-          <t>2020-07-10T01:55:41Z</t>
+          <t>2050</t>
         </is>
       </c>
       <c r="G115" t="inlineStr">
         <is>
-          <t>2049</t>
-        </is>
-      </c>
-      <c r="H115" t="inlineStr">
-        <is>
-          <t>85201</t>
+          <t>85231</t>
         </is>
       </c>
     </row>
@@ -4780,23 +4241,22 @@
           <t>Mathematics of Support Vector Machine | Soft Margin SVM</t>
         </is>
       </c>
-      <c r="D116" t="inlineStr"/>
-      <c r="E116" t="n">
+      <c r="D116" t="n">
         <v>878</v>
       </c>
+      <c r="E116" t="inlineStr">
+        <is>
+          <t>2020-08-07T05:50:18Z</t>
+        </is>
+      </c>
       <c r="F116" t="inlineStr">
         <is>
-          <t>2020-08-07T05:50:18Z</t>
+          <t>1139</t>
         </is>
       </c>
       <c r="G116" t="inlineStr">
         <is>
-          <t>1139</t>
-        </is>
-      </c>
-      <c r="H116" t="inlineStr">
-        <is>
-          <t>46081</t>
+          <t>46100</t>
         </is>
       </c>
     </row>
@@ -4814,27 +4274,22 @@
           <t>Kernel Trick in SVM | Code Example</t>
         </is>
       </c>
-      <c r="D117" t="inlineStr">
-        <is>
-          <t>['Education', 'Engineering', 'Campus', 'Placement', 'Skills', 'Machine Learning', 'Software', 'Web Development', 'Profile Building']</t>
-        </is>
-      </c>
-      <c r="E117" t="n">
+      <c r="D117" t="n">
         <v>844</v>
       </c>
+      <c r="E117" t="inlineStr">
+        <is>
+          <t>2020-08-07T05:54:13Z</t>
+        </is>
+      </c>
       <c r="F117" t="inlineStr">
         <is>
-          <t>2020-08-07T05:54:13Z</t>
+          <t>798</t>
         </is>
       </c>
       <c r="G117" t="inlineStr">
         <is>
-          <t>797</t>
-        </is>
-      </c>
-      <c r="H117" t="inlineStr">
-        <is>
-          <t>28581</t>
+          <t>28599</t>
         </is>
       </c>
     </row>
@@ -4852,23 +4307,22 @@
           <t>Kernel Trick in SVM | Geometric Intuition</t>
         </is>
       </c>
-      <c r="D118" t="inlineStr"/>
-      <c r="E118" t="n">
+      <c r="D118" t="n">
         <v>378</v>
       </c>
+      <c r="E118" t="inlineStr">
+        <is>
+          <t>2020-08-07T05:54:55Z</t>
+        </is>
+      </c>
       <c r="F118" t="inlineStr">
         <is>
-          <t>2020-08-07T05:54:55Z</t>
+          <t>888</t>
         </is>
       </c>
       <c r="G118" t="inlineStr">
         <is>
-          <t>888</t>
-        </is>
-      </c>
-      <c r="H118" t="inlineStr">
-        <is>
-          <t>36110</t>
+          <t>36127</t>
         </is>
       </c>
     </row>
@@ -4886,23 +4340,22 @@
           <t>Naive Bayes Classifier | Part 1 | Conditional Probability</t>
         </is>
       </c>
-      <c r="D119" t="inlineStr"/>
-      <c r="E119" t="n">
+      <c r="D119" t="n">
         <v>566</v>
       </c>
+      <c r="E119" t="inlineStr">
+        <is>
+          <t>2020-03-14T18:39:43Z</t>
+        </is>
+      </c>
       <c r="F119" t="inlineStr">
         <is>
-          <t>2020-03-14T18:39:43Z</t>
+          <t>787</t>
         </is>
       </c>
       <c r="G119" t="inlineStr">
         <is>
-          <t>787</t>
-        </is>
-      </c>
-      <c r="H119" t="inlineStr">
-        <is>
-          <t>51407</t>
+          <t>51434</t>
         </is>
       </c>
     </row>
@@ -4920,23 +4373,22 @@
           <t>Naive Bayes Classifier | Part 2 | Independent Events in Probability</t>
         </is>
       </c>
-      <c r="D120" t="inlineStr"/>
-      <c r="E120" t="n">
+      <c r="D120" t="n">
         <v>479</v>
       </c>
+      <c r="E120" t="inlineStr">
+        <is>
+          <t>2020-03-14T19:04:13Z</t>
+        </is>
+      </c>
       <c r="F120" t="inlineStr">
         <is>
-          <t>2020-03-14T19:04:13Z</t>
+          <t>432</t>
         </is>
       </c>
       <c r="G120" t="inlineStr">
         <is>
-          <t>432</t>
-        </is>
-      </c>
-      <c r="H120" t="inlineStr">
-        <is>
-          <t>20104</t>
+          <t>20112</t>
         </is>
       </c>
     </row>
@@ -4954,23 +4406,22 @@
           <t>Naive Bayes Classifier | Part 3 | Mutually Exclusive Events</t>
         </is>
       </c>
-      <c r="D121" t="inlineStr"/>
-      <c r="E121" t="n">
+      <c r="D121" t="n">
         <v>109</v>
       </c>
+      <c r="E121" t="inlineStr">
+        <is>
+          <t>2020-03-14T19:07:51Z</t>
+        </is>
+      </c>
       <c r="F121" t="inlineStr">
         <is>
-          <t>2020-03-14T19:07:51Z</t>
+          <t>286</t>
         </is>
       </c>
       <c r="G121" t="inlineStr">
         <is>
-          <t>286</t>
-        </is>
-      </c>
-      <c r="H121" t="inlineStr">
-        <is>
-          <t>16228</t>
+          <t>16237</t>
         </is>
       </c>
     </row>
@@ -4988,23 +4439,22 @@
           <t>Naive Bayes Classifier | Part 4 | Bayes Theorem in Probability</t>
         </is>
       </c>
-      <c r="D122" t="inlineStr"/>
-      <c r="E122" t="n">
+      <c r="D122" t="n">
         <v>267</v>
       </c>
+      <c r="E122" t="inlineStr">
+        <is>
+          <t>2020-03-14T19:21:02Z</t>
+        </is>
+      </c>
       <c r="F122" t="inlineStr">
         <is>
-          <t>2020-03-14T19:21:02Z</t>
+          <t>404</t>
         </is>
       </c>
       <c r="G122" t="inlineStr">
         <is>
-          <t>404</t>
-        </is>
-      </c>
-      <c r="H122" t="inlineStr">
-        <is>
-          <t>17467</t>
+          <t>17476</t>
         </is>
       </c>
     </row>
@@ -5022,23 +4472,22 @@
           <t>Naive Bayes Classifier | Part 5 | Problem based upon Bayes Theorem</t>
         </is>
       </c>
-      <c r="D123" t="inlineStr"/>
-      <c r="E123" t="n">
+      <c r="D123" t="n">
         <v>540</v>
       </c>
+      <c r="E123" t="inlineStr">
+        <is>
+          <t>2020-03-14T19:38:59Z</t>
+        </is>
+      </c>
       <c r="F123" t="inlineStr">
         <is>
-          <t>2020-03-14T19:38:59Z</t>
+          <t>421</t>
         </is>
       </c>
       <c r="G123" t="inlineStr">
         <is>
-          <t>421</t>
-        </is>
-      </c>
-      <c r="H123" t="inlineStr">
-        <is>
-          <t>18986</t>
+          <t>18991</t>
         </is>
       </c>
     </row>
@@ -5056,23 +4505,22 @@
           <t>Naive Bayes Classifier | Part 6 | Intuition</t>
         </is>
       </c>
-      <c r="D124" t="inlineStr"/>
-      <c r="E124" t="n">
+      <c r="D124" t="n">
         <v>884</v>
       </c>
+      <c r="E124" t="inlineStr">
+        <is>
+          <t>2020-03-14T20:17:23Z</t>
+        </is>
+      </c>
       <c r="F124" t="inlineStr">
         <is>
-          <t>2020-03-14T20:17:23Z</t>
+          <t>514</t>
         </is>
       </c>
       <c r="G124" t="inlineStr">
         <is>
-          <t>514</t>
-        </is>
-      </c>
-      <c r="H124" t="inlineStr">
-        <is>
-          <t>19500</t>
+          <t>19512</t>
         </is>
       </c>
     </row>
@@ -5090,23 +4538,22 @@
           <t>Naive Bayes Classifier | Part 7 | Mathematics behind Naive Bayes Algorithm</t>
         </is>
       </c>
-      <c r="D125" t="inlineStr"/>
-      <c r="E125" t="n">
+      <c r="D125" t="n">
         <v>1149</v>
       </c>
+      <c r="E125" t="inlineStr">
+        <is>
+          <t>2020-03-14T21:03:21Z</t>
+        </is>
+      </c>
       <c r="F125" t="inlineStr">
         <is>
-          <t>2020-03-14T21:03:21Z</t>
+          <t>516</t>
         </is>
       </c>
       <c r="G125" t="inlineStr">
         <is>
-          <t>516</t>
-        </is>
-      </c>
-      <c r="H125" t="inlineStr">
-        <is>
-          <t>18158</t>
+          <t>18174</t>
         </is>
       </c>
     </row>
@@ -5124,23 +4571,22 @@
           <t>Naive Bayes Classifier | Part 8 | Simple Example Code</t>
         </is>
       </c>
-      <c r="D126" t="inlineStr"/>
-      <c r="E126" t="n">
+      <c r="D126" t="n">
         <v>963</v>
       </c>
+      <c r="E126" t="inlineStr">
+        <is>
+          <t>2020-03-14T20:13:58Z</t>
+        </is>
+      </c>
       <c r="F126" t="inlineStr">
         <is>
-          <t>2020-03-14T20:13:58Z</t>
+          <t>468</t>
         </is>
       </c>
       <c r="G126" t="inlineStr">
         <is>
-          <t>468</t>
-        </is>
-      </c>
-      <c r="H126" t="inlineStr">
-        <is>
-          <t>19157</t>
+          <t>19165</t>
         </is>
       </c>
     </row>
@@ -5158,23 +4604,22 @@
           <t>Naive Bayes Part 9 | Handling Numerical Data</t>
         </is>
       </c>
-      <c r="D127" t="inlineStr"/>
-      <c r="E127" t="n">
+      <c r="D127" t="n">
         <v>527</v>
       </c>
+      <c r="E127" t="inlineStr">
+        <is>
+          <t>2020-04-27T05:38:31Z</t>
+        </is>
+      </c>
       <c r="F127" t="inlineStr">
         <is>
-          <t>2020-04-27T05:38:31Z</t>
+          <t>419</t>
         </is>
       </c>
       <c r="G127" t="inlineStr">
         <is>
-          <t>419</t>
-        </is>
-      </c>
-      <c r="H127" t="inlineStr">
-        <is>
-          <t>15211</t>
+          <t>15221</t>
         </is>
       </c>
     </row>
@@ -5192,27 +4637,22 @@
           <t>Introduction to XGBOOST | Machine Learning | CampusX</t>
         </is>
       </c>
-      <c r="D128" t="inlineStr">
-        <is>
-          <t>['Education', 'Engineering', 'Campus', 'Placement', 'Skills', 'Machine Learning', 'Software', 'Web Development', 'Profile Building']</t>
-        </is>
-      </c>
-      <c r="E128" t="n">
+      <c r="D128" t="n">
         <v>4777</v>
       </c>
+      <c r="E128" t="inlineStr">
+        <is>
+          <t>2023-10-14T10:47:05Z</t>
+        </is>
+      </c>
       <c r="F128" t="inlineStr">
         <is>
-          <t>2023-10-14T10:47:05Z</t>
+          <t>1308</t>
         </is>
       </c>
       <c r="G128" t="inlineStr">
         <is>
-          <t>1307</t>
-        </is>
-      </c>
-      <c r="H128" t="inlineStr">
-        <is>
-          <t>41454</t>
+          <t>41509</t>
         </is>
       </c>
     </row>
@@ -5230,27 +4670,22 @@
           <t>XGBoost for Regression | XGBoost Part 2 | CampusX</t>
         </is>
       </c>
-      <c r="D129" t="inlineStr">
-        <is>
-          <t>['Education', 'Engineering', 'Campus', 'Placement', 'Skills', 'Machine Learning', 'Software', 'Web Development', 'Profile Building']</t>
-        </is>
-      </c>
-      <c r="E129" t="n">
+      <c r="D129" t="n">
         <v>2837</v>
       </c>
+      <c r="E129" t="inlineStr">
+        <is>
+          <t>2023-10-24T12:58:03Z</t>
+        </is>
+      </c>
       <c r="F129" t="inlineStr">
         <is>
-          <t>2023-10-24T12:58:03Z</t>
+          <t>614</t>
         </is>
       </c>
       <c r="G129" t="inlineStr">
         <is>
-          <t>613</t>
-        </is>
-      </c>
-      <c r="H129" t="inlineStr">
-        <is>
-          <t>18904</t>
+          <t>18934</t>
         </is>
       </c>
     </row>
@@ -5268,27 +4703,22 @@
           <t>XGBoost For Classification | How XGBoost works on Classification Problems | CampusX</t>
         </is>
       </c>
-      <c r="D130" t="inlineStr">
-        <is>
-          <t>['Education', 'Engineering', 'Campus', 'Placement', 'Skills', 'Machine Learning', 'Software', 'Web Development', 'Profile Building', 'XGBoost', 'Classification', 'Predictive Modeling', 'Ensemble Learning', 'Data Science', 'XGBoost Tutorial', 'Classification Problems', 'Gradient Boosting', 'Decision Trees', 'Model Performance', 'Data Analysis', 'Predictive Analytics', 'Data Modeling']</t>
-        </is>
-      </c>
-      <c r="E130" t="n">
+      <c r="D130" t="n">
         <v>2348</v>
       </c>
+      <c r="E130" t="inlineStr">
+        <is>
+          <t>2023-11-12T03:14:03Z</t>
+        </is>
+      </c>
       <c r="F130" t="inlineStr">
         <is>
-          <t>2023-11-12T03:14:03Z</t>
+          <t>500</t>
         </is>
       </c>
       <c r="G130" t="inlineStr">
         <is>
-          <t>499</t>
-        </is>
-      </c>
-      <c r="H130" t="inlineStr">
-        <is>
-          <t>15588</t>
+          <t>15598</t>
         </is>
       </c>
     </row>
@@ -5306,27 +4736,22 @@
           <t>The Maths Behind XGBoost | Machine Learning | CampusX</t>
         </is>
       </c>
-      <c r="D131" t="inlineStr">
-        <is>
-          <t>['Education', 'Engineering', 'Campus', 'Placement', 'Skills', 'Machine Learning', 'Software', 'Profile Building', 'XGBoost', 'Extreme Gradient Boosting', 'Ensemble Learning', 'Machine Learning Algorithm', 'Gradient Boosting', 'Decision Trees', 'Classification', 'Regression', 'Ensemble Models', 'Predictive Modeling', 'Feature Importance', 'Regularization', 'Hyperparameter Tuning', 'Kaggle', 'Data Science', 'Scalable Machine Learning', 'Boosting Algorithm', 'Model Interpretability', 'XGBoost Tutorial', 'Model Performance', 'Cross-Validation']</t>
-        </is>
-      </c>
-      <c r="E131" t="n">
+      <c r="D131" t="n">
         <v>7048</v>
       </c>
+      <c r="E131" t="inlineStr">
+        <is>
+          <t>2023-12-02T05:46:28Z</t>
+        </is>
+      </c>
       <c r="F131" t="inlineStr">
         <is>
-          <t>2023-12-02T05:46:28Z</t>
+          <t>635</t>
         </is>
       </c>
       <c r="G131" t="inlineStr">
         <is>
-          <t>635</t>
-        </is>
-      </c>
-      <c r="H131" t="inlineStr">
-        <is>
-          <t>15629</t>
+          <t>15644</t>
         </is>
       </c>
     </row>
@@ -5344,27 +4769,22 @@
           <t>DBSCAN Clustering Algorithms | Density Based Clustering | How DBSCAN Works | CampusX</t>
         </is>
       </c>
-      <c r="D132" t="inlineStr">
-        <is>
-          <t>['Education', 'Engineering', 'Campus', 'Placement', 'Skills', 'Machine Learning', 'Software', 'Web Development']</t>
-        </is>
-      </c>
-      <c r="E132" t="n">
+      <c r="D132" t="n">
         <v>2056</v>
       </c>
+      <c r="E132" t="inlineStr">
+        <is>
+          <t>2023-12-17T00:29:03Z</t>
+        </is>
+      </c>
       <c r="F132" t="inlineStr">
         <is>
-          <t>2023-12-17T00:29:03Z</t>
+          <t>704</t>
         </is>
       </c>
       <c r="G132" t="inlineStr">
         <is>
-          <t>702</t>
-        </is>
-      </c>
-      <c r="H132" t="inlineStr">
-        <is>
-          <t>20232</t>
+          <t>20253</t>
         </is>
       </c>
     </row>
@@ -5382,27 +4802,22 @@
           <t>Imbalanced Data in Machine Learning | Undersampling | Oversampling | SMOTE</t>
         </is>
       </c>
-      <c r="D133" t="inlineStr">
-        <is>
-          <t>['Education', 'Engineering', 'Campus', 'Placement', 'Skills', 'Machine Learning', 'Software', 'Web Development', 'Profile Building']</t>
-        </is>
-      </c>
-      <c r="E133" t="n">
+      <c r="D133" t="n">
         <v>3437</v>
       </c>
+      <c r="E133" t="inlineStr">
+        <is>
+          <t>2024-05-04T09:29:32Z</t>
+        </is>
+      </c>
       <c r="F133" t="inlineStr">
         <is>
-          <t>2024-05-04T09:29:32Z</t>
+          <t>615</t>
         </is>
       </c>
       <c r="G133" t="inlineStr">
         <is>
-          <t>615</t>
-        </is>
-      </c>
-      <c r="H133" t="inlineStr">
-        <is>
-          <t>17679</t>
+          <t>17701</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
'publised_date' column is refined
</commit_message>
<xml_diff>
--- a/videoInformation.xlsx
+++ b/videoInformation.xlsx
@@ -484,17 +484,17 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>2021-03-13T16:15:53Z</t>
+          <t>2021-03-13</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>8993</t>
+          <t>8994</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>814498</t>
+          <t>814600</t>
         </is>
       </c>
     </row>
@@ -517,7 +517,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>2021-03-15T16:28:35Z</t>
+          <t>2021-03-15</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -550,7 +550,7 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>2021-03-16T13:49:16Z</t>
+          <t>2021-03-16</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -560,7 +560,7 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>183054</t>
+          <t>183089</t>
         </is>
       </c>
     </row>
@@ -583,7 +583,7 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>2021-03-17T14:13:41Z</t>
+          <t>2021-03-17</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -593,7 +593,7 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>120567</t>
+          <t>120571</t>
         </is>
       </c>
     </row>
@@ -616,7 +616,7 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>2021-03-18T12:41:31Z</t>
+          <t>2021-03-18</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -626,7 +626,7 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>103930</t>
+          <t>103970</t>
         </is>
       </c>
     </row>
@@ -649,17 +649,17 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>2021-03-19T13:34:29Z</t>
+          <t>2021-03-19</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>2800</t>
+          <t>2801</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>96692</t>
+          <t>96725</t>
         </is>
       </c>
     </row>
@@ -682,7 +682,7 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>2021-03-20T14:09:26Z</t>
+          <t>2021-03-20</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
@@ -692,7 +692,7 @@
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>85501</t>
+          <t>85505</t>
         </is>
       </c>
     </row>
@@ -715,17 +715,17 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>2021-03-22T14:14:44Z</t>
+          <t>2021-03-22</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>3585</t>
+          <t>3586</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>72238</t>
+          <t>72250</t>
         </is>
       </c>
     </row>
@@ -748,7 +748,7 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>2021-03-23T14:44:09Z</t>
+          <t>2021-03-23</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
@@ -758,7 +758,7 @@
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>86963</t>
+          <t>86973</t>
         </is>
       </c>
     </row>
@@ -781,7 +781,7 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>2021-03-24T12:49:59Z</t>
+          <t>2021-03-24</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
@@ -791,7 +791,7 @@
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>67414</t>
+          <t>67422</t>
         </is>
       </c>
     </row>
@@ -814,7 +814,7 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>2021-03-25T14:39:26Z</t>
+          <t>2021-03-25</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
@@ -847,7 +847,7 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>2021-03-26T15:47:45Z</t>
+          <t>2021-03-26</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
@@ -857,7 +857,7 @@
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>97728</t>
+          <t>97720</t>
         </is>
       </c>
     </row>
@@ -880,7 +880,7 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>2021-03-27T14:30:02Z</t>
+          <t>2021-03-27</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
@@ -913,7 +913,7 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>2021-03-29T14:30:01Z</t>
+          <t>2021-03-29</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
@@ -923,7 +923,7 @@
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>78585</t>
+          <t>78592</t>
         </is>
       </c>
     </row>
@@ -946,7 +946,7 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>2021-03-30T14:34:19Z</t>
+          <t>2021-03-30</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
@@ -956,7 +956,7 @@
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>100894</t>
+          <t>100893</t>
         </is>
       </c>
     </row>
@@ -979,17 +979,17 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>2021-03-31T14:30:04Z</t>
+          <t>2021-03-31</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>1952</t>
+          <t>1953</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>69183</t>
+          <t>69196</t>
         </is>
       </c>
     </row>
@@ -1012,17 +1012,17 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>2021-04-01T14:30:08Z</t>
+          <t>2021-04-01</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>3215</t>
+          <t>3217</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>106642</t>
+          <t>106658</t>
         </is>
       </c>
     </row>
@@ -1045,7 +1045,7 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>2021-04-02T15:12:18Z</t>
+          <t>2021-04-02</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
@@ -1055,7 +1055,7 @@
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>120135</t>
+          <t>120146</t>
         </is>
       </c>
     </row>
@@ -1078,7 +1078,7 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>2021-04-03T14:30:03Z</t>
+          <t>2021-04-03</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
@@ -1088,7 +1088,7 @@
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>79697</t>
+          <t>79698</t>
         </is>
       </c>
     </row>
@@ -1111,7 +1111,7 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>2021-04-05T14:30:00Z</t>
+          <t>2021-04-05</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
@@ -1121,7 +1121,7 @@
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>112125</t>
+          <t>112134</t>
         </is>
       </c>
     </row>
@@ -1144,7 +1144,7 @@
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>2021-04-06T14:30:00Z</t>
+          <t>2021-04-06</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
@@ -1154,7 +1154,7 @@
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>93061</t>
+          <t>93064</t>
         </is>
       </c>
     </row>
@@ -1177,7 +1177,7 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>2021-04-07T14:30:01Z</t>
+          <t>2021-04-07</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
@@ -1187,7 +1187,7 @@
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>64876</t>
+          <t>64877</t>
         </is>
       </c>
     </row>
@@ -1210,7 +1210,7 @@
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>2021-04-08T14:43:42Z</t>
+          <t>2021-04-08</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
@@ -1220,7 +1220,7 @@
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>130207</t>
+          <t>130209</t>
         </is>
       </c>
     </row>
@@ -1243,7 +1243,7 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>2021-04-09T14:32:00Z</t>
+          <t>2021-04-09</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
@@ -1253,7 +1253,7 @@
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>126114</t>
+          <t>126156</t>
         </is>
       </c>
     </row>
@@ -1276,7 +1276,7 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>2021-04-10T14:30:04Z</t>
+          <t>2021-04-10</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
@@ -1286,7 +1286,7 @@
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>92298</t>
+          <t>92300</t>
         </is>
       </c>
     </row>
@@ -1309,7 +1309,7 @@
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>2021-04-12T16:55:33Z</t>
+          <t>2021-04-12</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
@@ -1342,17 +1342,17 @@
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>2021-04-13T14:30:05Z</t>
+          <t>2021-04-13</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>2674</t>
+          <t>2675</t>
         </is>
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>107602</t>
+          <t>107620</t>
         </is>
       </c>
     </row>
@@ -1375,7 +1375,7 @@
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>2021-04-14T14:30:00Z</t>
+          <t>2021-04-14</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
@@ -1408,7 +1408,7 @@
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>2021-04-15T15:00:41Z</t>
+          <t>2021-04-15</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
@@ -1441,7 +1441,7 @@
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>2021-04-16T14:38:42Z</t>
+          <t>2021-04-16</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
@@ -1474,17 +1474,17 @@
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>2021-04-17T14:30:05Z</t>
+          <t>2021-04-17</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>1724</t>
+          <t>1725</t>
         </is>
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>57078</t>
+          <t>57089</t>
         </is>
       </c>
     </row>
@@ -1507,7 +1507,7 @@
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>2021-04-19T14:28:16Z</t>
+          <t>2021-04-19</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
@@ -1517,7 +1517,7 @@
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>55764</t>
+          <t>55766</t>
         </is>
       </c>
     </row>
@@ -1540,7 +1540,7 @@
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>2021-04-20T14:30:00Z</t>
+          <t>2021-04-20</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
@@ -1550,7 +1550,7 @@
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>37296</t>
+          <t>37304</t>
         </is>
       </c>
     </row>
@@ -1573,7 +1573,7 @@
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>2021-04-21T14:30:01Z</t>
+          <t>2021-04-21</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
@@ -1606,7 +1606,7 @@
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>2021-04-22T14:30:00Z</t>
+          <t>2021-04-22</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
@@ -1616,7 +1616,7 @@
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>63868</t>
+          <t>63872</t>
         </is>
       </c>
     </row>
@@ -1639,17 +1639,17 @@
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>2021-04-23T14:30:13Z</t>
+          <t>2021-04-23</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>1454</t>
+          <t>1455</t>
         </is>
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>57119</t>
+          <t>57136</t>
         </is>
       </c>
     </row>
@@ -1672,7 +1672,7 @@
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>2021-04-24T14:30:10Z</t>
+          <t>2021-04-24</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
@@ -1705,7 +1705,7 @@
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>2021-04-26T14:30:02Z</t>
+          <t>2021-04-26</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
@@ -1715,7 +1715,7 @@
       </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t>44374</t>
+          <t>44368</t>
         </is>
       </c>
     </row>
@@ -1738,7 +1738,7 @@
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>2021-04-27T14:30:01Z</t>
+          <t>2021-04-27</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
@@ -1748,7 +1748,7 @@
       </c>
       <c r="G40" t="inlineStr">
         <is>
-          <t>47530</t>
+          <t>47529</t>
         </is>
       </c>
     </row>
@@ -1771,7 +1771,7 @@
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>2021-04-28T14:30:01Z</t>
+          <t>2021-04-28</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
@@ -1781,7 +1781,7 @@
       </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t>35671</t>
+          <t>35675</t>
         </is>
       </c>
     </row>
@@ -1804,7 +1804,7 @@
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>2021-04-29T14:30:11Z</t>
+          <t>2021-04-29</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
@@ -1814,7 +1814,7 @@
       </c>
       <c r="G42" t="inlineStr">
         <is>
-          <t>58957</t>
+          <t>58955</t>
         </is>
       </c>
     </row>
@@ -1837,17 +1837,17 @@
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>2021-04-30T14:30:04Z</t>
+          <t>2021-04-30</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>1231</t>
+          <t>1232</t>
         </is>
       </c>
       <c r="G43" t="inlineStr">
         <is>
-          <t>51449</t>
+          <t>51462</t>
         </is>
       </c>
     </row>
@@ -1870,17 +1870,17 @@
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>2021-05-01T14:30:01Z</t>
+          <t>2021-05-01</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>1325</t>
+          <t>1326</t>
         </is>
       </c>
       <c r="G44" t="inlineStr">
         <is>
-          <t>55510</t>
+          <t>55526</t>
         </is>
       </c>
     </row>
@@ -1903,7 +1903,7 @@
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>2021-05-03T14:30:04Z</t>
+          <t>2021-05-03</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
@@ -1913,7 +1913,7 @@
       </c>
       <c r="G45" t="inlineStr">
         <is>
-          <t>32840</t>
+          <t>32849</t>
         </is>
       </c>
     </row>
@@ -1936,7 +1936,7 @@
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>2021-05-04T14:30:09Z</t>
+          <t>2021-05-04</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
@@ -1946,7 +1946,7 @@
       </c>
       <c r="G46" t="inlineStr">
         <is>
-          <t>33955</t>
+          <t>33969</t>
         </is>
       </c>
     </row>
@@ -1969,7 +1969,7 @@
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>2021-05-05T14:30:03Z</t>
+          <t>2021-05-05</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
@@ -1979,7 +1979,7 @@
       </c>
       <c r="G47" t="inlineStr">
         <is>
-          <t>50718</t>
+          <t>50728</t>
         </is>
       </c>
     </row>
@@ -2002,7 +2002,7 @@
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>2021-05-06T14:30:03Z</t>
+          <t>2021-05-06</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
@@ -2012,7 +2012,7 @@
       </c>
       <c r="G48" t="inlineStr">
         <is>
-          <t>96601</t>
+          <t>96610</t>
         </is>
       </c>
     </row>
@@ -2035,7 +2035,7 @@
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>2021-05-07T14:30:04Z</t>
+          <t>2021-05-07</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
@@ -2045,7 +2045,7 @@
       </c>
       <c r="G49" t="inlineStr">
         <is>
-          <t>79865</t>
+          <t>79883</t>
         </is>
       </c>
     </row>
@@ -2068,17 +2068,17 @@
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>2021-05-08T14:30:06Z</t>
+          <t>2021-05-08</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>1468</t>
+          <t>1469</t>
         </is>
       </c>
       <c r="G50" t="inlineStr">
         <is>
-          <t>51135</t>
+          <t>51140</t>
         </is>
       </c>
     </row>
@@ -2101,7 +2101,7 @@
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>2021-05-10T14:30:07Z</t>
+          <t>2021-05-10</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
@@ -2134,7 +2134,7 @@
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>2021-05-11T14:30:06Z</t>
+          <t>2021-05-11</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
@@ -2167,7 +2167,7 @@
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>2021-05-13T14:30:02Z</t>
+          <t>2021-05-13</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
@@ -2200,7 +2200,7 @@
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>2021-05-14T14:30:01Z</t>
+          <t>2021-05-14</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
@@ -2233,7 +2233,7 @@
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>2021-05-15T14:30:07Z</t>
+          <t>2021-05-15</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
@@ -2266,7 +2266,7 @@
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>2021-05-17T14:30:03Z</t>
+          <t>2021-05-17</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
@@ -2299,7 +2299,7 @@
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>2021-05-21T14:30:01Z</t>
+          <t>2021-05-21</t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
@@ -2309,7 +2309,7 @@
       </c>
       <c r="G57" t="inlineStr">
         <is>
-          <t>161453</t>
+          <t>161461</t>
         </is>
       </c>
     </row>
@@ -2332,7 +2332,7 @@
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>2021-05-22T14:35:24Z</t>
+          <t>2021-05-22</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
@@ -2365,7 +2365,7 @@
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>2021-05-25T14:30:06Z</t>
+          <t>2021-05-25</t>
         </is>
       </c>
       <c r="F59" t="inlineStr">
@@ -2398,7 +2398,7 @@
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>2021-05-26T14:30:12Z</t>
+          <t>2021-05-26</t>
         </is>
       </c>
       <c r="F60" t="inlineStr">
@@ -2431,7 +2431,7 @@
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>2021-05-29T01:48:09Z</t>
+          <t>2021-05-29</t>
         </is>
       </c>
       <c r="F61" t="inlineStr">
@@ -2441,7 +2441,7 @@
       </c>
       <c r="G61" t="inlineStr">
         <is>
-          <t>60712</t>
+          <t>60728</t>
         </is>
       </c>
     </row>
@@ -2464,17 +2464,17 @@
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>2020-06-05T19:54:56Z</t>
+          <t>2020-06-05</t>
         </is>
       </c>
       <c r="F62" t="inlineStr">
         <is>
-          <t>1561</t>
+          <t>1563</t>
         </is>
       </c>
       <c r="G62" t="inlineStr">
         <is>
-          <t>63805</t>
+          <t>63821</t>
         </is>
       </c>
     </row>
@@ -2497,7 +2497,7 @@
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>2021-06-02T14:30:02Z</t>
+          <t>2021-06-02</t>
         </is>
       </c>
       <c r="F63" t="inlineStr">
@@ -2507,7 +2507,7 @@
       </c>
       <c r="G63" t="inlineStr">
         <is>
-          <t>77738</t>
+          <t>77747</t>
         </is>
       </c>
     </row>
@@ -2530,7 +2530,7 @@
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>2021-06-03T14:30:05Z</t>
+          <t>2021-06-03</t>
         </is>
       </c>
       <c r="F64" t="inlineStr">
@@ -2563,7 +2563,7 @@
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>2021-06-04T14:30:02Z</t>
+          <t>2021-06-04</t>
         </is>
       </c>
       <c r="F65" t="inlineStr">
@@ -2596,7 +2596,7 @@
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>2021-06-08T08:42:26Z</t>
+          <t>2021-06-08</t>
         </is>
       </c>
       <c r="F66" t="inlineStr">
@@ -2629,7 +2629,7 @@
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>2021-06-10T14:30:03Z</t>
+          <t>2021-06-10</t>
         </is>
       </c>
       <c r="F67" t="inlineStr">
@@ -2662,7 +2662,7 @@
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>2021-06-11T14:30:02Z</t>
+          <t>2021-06-11</t>
         </is>
       </c>
       <c r="F68" t="inlineStr">
@@ -2695,7 +2695,7 @@
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>2021-06-12T14:30:01Z</t>
+          <t>2021-06-12</t>
         </is>
       </c>
       <c r="F69" t="inlineStr">
@@ -2728,17 +2728,17 @@
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>2021-06-15T14:30:10Z</t>
+          <t>2021-06-15</t>
         </is>
       </c>
       <c r="F70" t="inlineStr">
         <is>
-          <t>2012</t>
+          <t>2013</t>
         </is>
       </c>
       <c r="G70" t="inlineStr">
         <is>
-          <t>113359</t>
+          <t>113371</t>
         </is>
       </c>
     </row>
@@ -2761,7 +2761,7 @@
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>2021-06-16T14:30:08Z</t>
+          <t>2021-06-16</t>
         </is>
       </c>
       <c r="F71" t="inlineStr">
@@ -2794,7 +2794,7 @@
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>2021-06-17T14:30:04Z</t>
+          <t>2021-06-17</t>
         </is>
       </c>
       <c r="F72" t="inlineStr">
@@ -2827,7 +2827,7 @@
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>2021-06-18T14:30:04Z</t>
+          <t>2021-06-18</t>
         </is>
       </c>
       <c r="F73" t="inlineStr">
@@ -2860,7 +2860,7 @@
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>2021-06-19T09:49:04Z</t>
+          <t>2021-06-19</t>
         </is>
       </c>
       <c r="F74" t="inlineStr">
@@ -2893,7 +2893,7 @@
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>2021-06-21T14:30:01Z</t>
+          <t>2021-06-21</t>
         </is>
       </c>
       <c r="F75" t="inlineStr">
@@ -2903,7 +2903,7 @@
       </c>
       <c r="G75" t="inlineStr">
         <is>
-          <t>44086</t>
+          <t>44102</t>
         </is>
       </c>
     </row>
@@ -2926,17 +2926,17 @@
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>2021-06-23T14:30:05Z</t>
+          <t>2021-06-23</t>
         </is>
       </c>
       <c r="F76" t="inlineStr">
         <is>
-          <t>1245</t>
+          <t>1246</t>
         </is>
       </c>
       <c r="G76" t="inlineStr">
         <is>
-          <t>58905</t>
+          <t>58919</t>
         </is>
       </c>
     </row>
@@ -2959,7 +2959,7 @@
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>2021-06-24T14:30:16Z</t>
+          <t>2021-06-24</t>
         </is>
       </c>
       <c r="F77" t="inlineStr">
@@ -2992,7 +2992,7 @@
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>2021-06-28T14:30:03Z</t>
+          <t>2021-06-28</t>
         </is>
       </c>
       <c r="F78" t="inlineStr">
@@ -3002,7 +3002,7 @@
       </c>
       <c r="G78" t="inlineStr">
         <is>
-          <t>39884</t>
+          <t>39895</t>
         </is>
       </c>
     </row>
@@ -3025,7 +3025,7 @@
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>2021-06-29T14:30:05Z</t>
+          <t>2021-06-29</t>
         </is>
       </c>
       <c r="F79" t="inlineStr">
@@ -3058,7 +3058,7 @@
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>2021-06-30T14:30:00Z</t>
+          <t>2021-06-30</t>
         </is>
       </c>
       <c r="F80" t="inlineStr">
@@ -3091,7 +3091,7 @@
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>2021-07-02T14:30:01Z</t>
+          <t>2021-07-02</t>
         </is>
       </c>
       <c r="F81" t="inlineStr">
@@ -3101,7 +3101,7 @@
       </c>
       <c r="G81" t="inlineStr">
         <is>
-          <t>93917</t>
+          <t>93946</t>
         </is>
       </c>
     </row>
@@ -3124,7 +3124,7 @@
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>2021-07-03T14:30:06Z</t>
+          <t>2021-07-03</t>
         </is>
       </c>
       <c r="F82" t="inlineStr">
@@ -3157,7 +3157,7 @@
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>2021-07-05T14:30:09Z</t>
+          <t>2021-07-05</t>
         </is>
       </c>
       <c r="F83" t="inlineStr">
@@ -3167,7 +3167,7 @@
       </c>
       <c r="G83" t="inlineStr">
         <is>
-          <t>32219</t>
+          <t>32229</t>
         </is>
       </c>
     </row>
@@ -3190,7 +3190,7 @@
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>2021-03-19T13:49:09Z</t>
+          <t>2021-03-19</t>
         </is>
       </c>
       <c r="F84" t="inlineStr">
@@ -3223,17 +3223,17 @@
       </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t>2021-07-12T14:30:15Z</t>
+          <t>2021-07-12</t>
         </is>
       </c>
       <c r="F85" t="inlineStr">
         <is>
-          <t>2096</t>
+          <t>2097</t>
         </is>
       </c>
       <c r="G85" t="inlineStr">
         <is>
-          <t>75639</t>
+          <t>75656</t>
         </is>
       </c>
     </row>
@@ -3256,7 +3256,7 @@
       </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t>2021-03-09T13:17:07Z</t>
+          <t>2021-03-09</t>
         </is>
       </c>
       <c r="F86" t="inlineStr">
@@ -3289,7 +3289,7 @@
       </c>
       <c r="E87" t="inlineStr">
         <is>
-          <t>2021-03-10T14:13:57Z</t>
+          <t>2021-03-10</t>
         </is>
       </c>
       <c r="F87" t="inlineStr">
@@ -3322,7 +3322,7 @@
       </c>
       <c r="E88" t="inlineStr">
         <is>
-          <t>2021-03-11T14:06:31Z</t>
+          <t>2021-03-11</t>
         </is>
       </c>
       <c r="F88" t="inlineStr">
@@ -3355,17 +3355,17 @@
       </c>
       <c r="E89" t="inlineStr">
         <is>
-          <t>2021-03-12T15:25:14Z</t>
+          <t>2021-03-12</t>
         </is>
       </c>
       <c r="F89" t="inlineStr">
         <is>
-          <t>1235</t>
+          <t>1236</t>
         </is>
       </c>
       <c r="G89" t="inlineStr">
         <is>
-          <t>45550</t>
+          <t>45565</t>
         </is>
       </c>
     </row>
@@ -3388,17 +3388,17 @@
       </c>
       <c r="E90" t="inlineStr">
         <is>
-          <t>2021-03-16T13:37:35Z</t>
+          <t>2021-03-16</t>
         </is>
       </c>
       <c r="F90" t="inlineStr">
         <is>
-          <t>932</t>
+          <t>933</t>
         </is>
       </c>
       <c r="G90" t="inlineStr">
         <is>
-          <t>26720</t>
+          <t>26728</t>
         </is>
       </c>
     </row>
@@ -3421,7 +3421,7 @@
       </c>
       <c r="E91" t="inlineStr">
         <is>
-          <t>2021-03-17T19:49:37Z</t>
+          <t>2021-03-17</t>
         </is>
       </c>
       <c r="F91" t="inlineStr">
@@ -3431,7 +3431,7 @@
       </c>
       <c r="G91" t="inlineStr">
         <is>
-          <t>19391</t>
+          <t>19396</t>
         </is>
       </c>
     </row>
@@ -3454,7 +3454,7 @@
       </c>
       <c r="E92" t="inlineStr">
         <is>
-          <t>2021-07-19T15:13:28Z</t>
+          <t>2021-07-19</t>
         </is>
       </c>
       <c r="F92" t="inlineStr">
@@ -3464,7 +3464,7 @@
       </c>
       <c r="G92" t="inlineStr">
         <is>
-          <t>54143</t>
+          <t>54156</t>
         </is>
       </c>
     </row>
@@ -3487,7 +3487,7 @@
       </c>
       <c r="E93" t="inlineStr">
         <is>
-          <t>2021-07-20T14:30:08Z</t>
+          <t>2021-07-20</t>
         </is>
       </c>
       <c r="F93" t="inlineStr">
@@ -3497,7 +3497,7 @@
       </c>
       <c r="G93" t="inlineStr">
         <is>
-          <t>27511</t>
+          <t>27522</t>
         </is>
       </c>
     </row>
@@ -3520,7 +3520,7 @@
       </c>
       <c r="E94" t="inlineStr">
         <is>
-          <t>2021-07-22T14:30:06Z</t>
+          <t>2021-07-22</t>
         </is>
       </c>
       <c r="F94" t="inlineStr">
@@ -3553,7 +3553,7 @@
       </c>
       <c r="E95" t="inlineStr">
         <is>
-          <t>2021-07-23T14:30:05Z</t>
+          <t>2021-07-23</t>
         </is>
       </c>
       <c r="F95" t="inlineStr">
@@ -3586,7 +3586,7 @@
       </c>
       <c r="E96" t="inlineStr">
         <is>
-          <t>2021-07-26T14:30:01Z</t>
+          <t>2021-07-26</t>
         </is>
       </c>
       <c r="F96" t="inlineStr">
@@ -3619,7 +3619,7 @@
       </c>
       <c r="E97" t="inlineStr">
         <is>
-          <t>2021-07-28T14:30:08Z</t>
+          <t>2021-07-28</t>
         </is>
       </c>
       <c r="F97" t="inlineStr">
@@ -3652,7 +3652,7 @@
       </c>
       <c r="E98" t="inlineStr">
         <is>
-          <t>2021-07-30T14:30:04Z</t>
+          <t>2021-07-30</t>
         </is>
       </c>
       <c r="F98" t="inlineStr">
@@ -3662,7 +3662,7 @@
       </c>
       <c r="G98" t="inlineStr">
         <is>
-          <t>35772</t>
+          <t>35777</t>
         </is>
       </c>
     </row>
@@ -3685,7 +3685,7 @@
       </c>
       <c r="E99" t="inlineStr">
         <is>
-          <t>2021-08-09T14:30:15Z</t>
+          <t>2021-08-09</t>
         </is>
       </c>
       <c r="F99" t="inlineStr">
@@ -3718,7 +3718,7 @@
       </c>
       <c r="E100" t="inlineStr">
         <is>
-          <t>2021-08-10T14:30:10Z</t>
+          <t>2021-08-10</t>
         </is>
       </c>
       <c r="F100" t="inlineStr">
@@ -3751,7 +3751,7 @@
       </c>
       <c r="E101" t="inlineStr">
         <is>
-          <t>2021-08-16T14:30:00Z</t>
+          <t>2021-08-16</t>
         </is>
       </c>
       <c r="F101" t="inlineStr">
@@ -3784,7 +3784,7 @@
       </c>
       <c r="E102" t="inlineStr">
         <is>
-          <t>2021-08-17T14:30:02Z</t>
+          <t>2021-08-17</t>
         </is>
       </c>
       <c r="F102" t="inlineStr">
@@ -3794,7 +3794,7 @@
       </c>
       <c r="G102" t="inlineStr">
         <is>
-          <t>18633</t>
+          <t>18638</t>
         </is>
       </c>
     </row>
@@ -3817,7 +3817,7 @@
       </c>
       <c r="E103" t="inlineStr">
         <is>
-          <t>2021-08-18T14:30:01Z</t>
+          <t>2021-08-18</t>
         </is>
       </c>
       <c r="F103" t="inlineStr">
@@ -3827,7 +3827,7 @@
       </c>
       <c r="G103" t="inlineStr">
         <is>
-          <t>33270</t>
+          <t>33274</t>
         </is>
       </c>
     </row>
@@ -3850,7 +3850,7 @@
       </c>
       <c r="E104" t="inlineStr">
         <is>
-          <t>2021-08-24T14:30:01Z</t>
+          <t>2021-08-24</t>
         </is>
       </c>
       <c r="F104" t="inlineStr">
@@ -3860,7 +3860,7 @@
       </c>
       <c r="G104" t="inlineStr">
         <is>
-          <t>84638</t>
+          <t>84643</t>
         </is>
       </c>
     </row>
@@ -3883,7 +3883,7 @@
       </c>
       <c r="E105" t="inlineStr">
         <is>
-          <t>2021-08-26T14:30:11Z</t>
+          <t>2021-08-26</t>
         </is>
       </c>
       <c r="F105" t="inlineStr">
@@ -3893,7 +3893,7 @@
       </c>
       <c r="G105" t="inlineStr">
         <is>
-          <t>53017</t>
+          <t>53027</t>
         </is>
       </c>
     </row>
@@ -3916,7 +3916,7 @@
       </c>
       <c r="E106" t="inlineStr">
         <is>
-          <t>2021-08-25T14:30:02Z</t>
+          <t>2021-08-25</t>
         </is>
       </c>
       <c r="F106" t="inlineStr">
@@ -3926,7 +3926,7 @@
       </c>
       <c r="G106" t="inlineStr">
         <is>
-          <t>37758</t>
+          <t>37762</t>
         </is>
       </c>
     </row>
@@ -3949,7 +3949,7 @@
       </c>
       <c r="E107" t="inlineStr">
         <is>
-          <t>2021-09-09T13:30:13Z</t>
+          <t>2021-09-09</t>
         </is>
       </c>
       <c r="F107" t="inlineStr">
@@ -3959,7 +3959,7 @@
       </c>
       <c r="G107" t="inlineStr">
         <is>
-          <t>61921</t>
+          <t>61930</t>
         </is>
       </c>
     </row>
@@ -3982,7 +3982,7 @@
       </c>
       <c r="E108" t="inlineStr">
         <is>
-          <t>2021-09-20T13:30:19Z</t>
+          <t>2021-09-20</t>
         </is>
       </c>
       <c r="F108" t="inlineStr">
@@ -3992,7 +3992,7 @@
       </c>
       <c r="G108" t="inlineStr">
         <is>
-          <t>30418</t>
+          <t>30421</t>
         </is>
       </c>
     </row>
@@ -4015,7 +4015,7 @@
       </c>
       <c r="E109" t="inlineStr">
         <is>
-          <t>2023-08-08T14:00:04Z</t>
+          <t>2023-08-08</t>
         </is>
       </c>
       <c r="F109" t="inlineStr">
@@ -4025,7 +4025,7 @@
       </c>
       <c r="G109" t="inlineStr">
         <is>
-          <t>25999</t>
+          <t>26008</t>
         </is>
       </c>
     </row>
@@ -4048,7 +4048,7 @@
       </c>
       <c r="E110" t="inlineStr">
         <is>
-          <t>2021-09-30T13:30:09Z</t>
+          <t>2021-09-30</t>
         </is>
       </c>
       <c r="F110" t="inlineStr">
@@ -4058,7 +4058,7 @@
       </c>
       <c r="G110" t="inlineStr">
         <is>
-          <t>22812</t>
+          <t>22814</t>
         </is>
       </c>
     </row>
@@ -4081,7 +4081,7 @@
       </c>
       <c r="E111" t="inlineStr">
         <is>
-          <t>2021-11-07T14:00:06Z</t>
+          <t>2021-11-07</t>
         </is>
       </c>
       <c r="F111" t="inlineStr">
@@ -4091,7 +4091,7 @@
       </c>
       <c r="G111" t="inlineStr">
         <is>
-          <t>38089</t>
+          <t>38093</t>
         </is>
       </c>
     </row>
@@ -4114,7 +4114,7 @@
       </c>
       <c r="E112" t="inlineStr">
         <is>
-          <t>2023-05-23T16:00:11Z</t>
+          <t>2023-05-23</t>
         </is>
       </c>
       <c r="F112" t="inlineStr">
@@ -4124,7 +4124,7 @@
       </c>
       <c r="G112" t="inlineStr">
         <is>
-          <t>49968</t>
+          <t>49990</t>
         </is>
       </c>
     </row>
@@ -4147,7 +4147,7 @@
       </c>
       <c r="E113" t="inlineStr">
         <is>
-          <t>2022-06-20T14:00:07Z</t>
+          <t>2022-06-20</t>
         </is>
       </c>
       <c r="F113" t="inlineStr">
@@ -4157,7 +4157,7 @@
       </c>
       <c r="G113" t="inlineStr">
         <is>
-          <t>46567</t>
+          <t>46582</t>
         </is>
       </c>
     </row>
@@ -4180,17 +4180,17 @@
       </c>
       <c r="E114" t="inlineStr">
         <is>
-          <t>2020-07-10T01:54:27Z</t>
+          <t>2020-07-10</t>
         </is>
       </c>
       <c r="F114" t="inlineStr">
         <is>
-          <t>1815</t>
+          <t>1816</t>
         </is>
       </c>
       <c r="G114" t="inlineStr">
         <is>
-          <t>98578</t>
+          <t>98588</t>
         </is>
       </c>
     </row>
@@ -4213,7 +4213,7 @@
       </c>
       <c r="E115" t="inlineStr">
         <is>
-          <t>2020-07-10T01:55:41Z</t>
+          <t>2020-07-10</t>
         </is>
       </c>
       <c r="F115" t="inlineStr">
@@ -4223,7 +4223,7 @@
       </c>
       <c r="G115" t="inlineStr">
         <is>
-          <t>85231</t>
+          <t>85257</t>
         </is>
       </c>
     </row>
@@ -4246,7 +4246,7 @@
       </c>
       <c r="E116" t="inlineStr">
         <is>
-          <t>2020-08-07T05:50:18Z</t>
+          <t>2020-08-07</t>
         </is>
       </c>
       <c r="F116" t="inlineStr">
@@ -4256,7 +4256,7 @@
       </c>
       <c r="G116" t="inlineStr">
         <is>
-          <t>46100</t>
+          <t>46102</t>
         </is>
       </c>
     </row>
@@ -4279,7 +4279,7 @@
       </c>
       <c r="E117" t="inlineStr">
         <is>
-          <t>2020-08-07T05:54:13Z</t>
+          <t>2020-08-07</t>
         </is>
       </c>
       <c r="F117" t="inlineStr">
@@ -4289,7 +4289,7 @@
       </c>
       <c r="G117" t="inlineStr">
         <is>
-          <t>28599</t>
+          <t>28609</t>
         </is>
       </c>
     </row>
@@ -4312,7 +4312,7 @@
       </c>
       <c r="E118" t="inlineStr">
         <is>
-          <t>2020-08-07T05:54:55Z</t>
+          <t>2020-08-07</t>
         </is>
       </c>
       <c r="F118" t="inlineStr">
@@ -4322,7 +4322,7 @@
       </c>
       <c r="G118" t="inlineStr">
         <is>
-          <t>36127</t>
+          <t>36139</t>
         </is>
       </c>
     </row>
@@ -4345,7 +4345,7 @@
       </c>
       <c r="E119" t="inlineStr">
         <is>
-          <t>2020-03-14T18:39:43Z</t>
+          <t>2020-03-14</t>
         </is>
       </c>
       <c r="F119" t="inlineStr">
@@ -4355,7 +4355,7 @@
       </c>
       <c r="G119" t="inlineStr">
         <is>
-          <t>51434</t>
+          <t>51430</t>
         </is>
       </c>
     </row>
@@ -4378,7 +4378,7 @@
       </c>
       <c r="E120" t="inlineStr">
         <is>
-          <t>2020-03-14T19:04:13Z</t>
+          <t>2020-03-14</t>
         </is>
       </c>
       <c r="F120" t="inlineStr">
@@ -4388,7 +4388,7 @@
       </c>
       <c r="G120" t="inlineStr">
         <is>
-          <t>20112</t>
+          <t>20114</t>
         </is>
       </c>
     </row>
@@ -4411,7 +4411,7 @@
       </c>
       <c r="E121" t="inlineStr">
         <is>
-          <t>2020-03-14T19:07:51Z</t>
+          <t>2020-03-14</t>
         </is>
       </c>
       <c r="F121" t="inlineStr">
@@ -4444,7 +4444,7 @@
       </c>
       <c r="E122" t="inlineStr">
         <is>
-          <t>2020-03-14T19:21:02Z</t>
+          <t>2020-03-14</t>
         </is>
       </c>
       <c r="F122" t="inlineStr">
@@ -4477,7 +4477,7 @@
       </c>
       <c r="E123" t="inlineStr">
         <is>
-          <t>2020-03-14T19:38:59Z</t>
+          <t>2020-03-14</t>
         </is>
       </c>
       <c r="F123" t="inlineStr">
@@ -4487,7 +4487,7 @@
       </c>
       <c r="G123" t="inlineStr">
         <is>
-          <t>18991</t>
+          <t>18993</t>
         </is>
       </c>
     </row>
@@ -4510,7 +4510,7 @@
       </c>
       <c r="E124" t="inlineStr">
         <is>
-          <t>2020-03-14T20:17:23Z</t>
+          <t>2020-03-14</t>
         </is>
       </c>
       <c r="F124" t="inlineStr">
@@ -4543,7 +4543,7 @@
       </c>
       <c r="E125" t="inlineStr">
         <is>
-          <t>2020-03-14T21:03:21Z</t>
+          <t>2020-03-14</t>
         </is>
       </c>
       <c r="F125" t="inlineStr">
@@ -4576,7 +4576,7 @@
       </c>
       <c r="E126" t="inlineStr">
         <is>
-          <t>2020-03-14T20:13:58Z</t>
+          <t>2020-03-14</t>
         </is>
       </c>
       <c r="F126" t="inlineStr">
@@ -4609,7 +4609,7 @@
       </c>
       <c r="E127" t="inlineStr">
         <is>
-          <t>2020-04-27T05:38:31Z</t>
+          <t>2020-04-27</t>
         </is>
       </c>
       <c r="F127" t="inlineStr">
@@ -4642,17 +4642,17 @@
       </c>
       <c r="E128" t="inlineStr">
         <is>
-          <t>2023-10-14T10:47:05Z</t>
+          <t>2023-10-14</t>
         </is>
       </c>
       <c r="F128" t="inlineStr">
         <is>
-          <t>1308</t>
+          <t>1307</t>
         </is>
       </c>
       <c r="G128" t="inlineStr">
         <is>
-          <t>41509</t>
+          <t>41508</t>
         </is>
       </c>
     </row>
@@ -4675,7 +4675,7 @@
       </c>
       <c r="E129" t="inlineStr">
         <is>
-          <t>2023-10-24T12:58:03Z</t>
+          <t>2023-10-24</t>
         </is>
       </c>
       <c r="F129" t="inlineStr">
@@ -4685,7 +4685,7 @@
       </c>
       <c r="G129" t="inlineStr">
         <is>
-          <t>18934</t>
+          <t>18935</t>
         </is>
       </c>
     </row>
@@ -4708,7 +4708,7 @@
       </c>
       <c r="E130" t="inlineStr">
         <is>
-          <t>2023-11-12T03:14:03Z</t>
+          <t>2023-11-12</t>
         </is>
       </c>
       <c r="F130" t="inlineStr">
@@ -4718,7 +4718,7 @@
       </c>
       <c r="G130" t="inlineStr">
         <is>
-          <t>15598</t>
+          <t>15606</t>
         </is>
       </c>
     </row>
@@ -4741,17 +4741,17 @@
       </c>
       <c r="E131" t="inlineStr">
         <is>
-          <t>2023-12-02T05:46:28Z</t>
+          <t>2023-12-02</t>
         </is>
       </c>
       <c r="F131" t="inlineStr">
         <is>
-          <t>635</t>
+          <t>636</t>
         </is>
       </c>
       <c r="G131" t="inlineStr">
         <is>
-          <t>15644</t>
+          <t>15652</t>
         </is>
       </c>
     </row>
@@ -4774,7 +4774,7 @@
       </c>
       <c r="E132" t="inlineStr">
         <is>
-          <t>2023-12-17T00:29:03Z</t>
+          <t>2023-12-17</t>
         </is>
       </c>
       <c r="F132" t="inlineStr">
@@ -4784,7 +4784,7 @@
       </c>
       <c r="G132" t="inlineStr">
         <is>
-          <t>20253</t>
+          <t>20258</t>
         </is>
       </c>
     </row>
@@ -4807,7 +4807,7 @@
       </c>
       <c r="E133" t="inlineStr">
         <is>
-          <t>2024-05-04T09:29:32Z</t>
+          <t>2024-05-04</t>
         </is>
       </c>
       <c r="F133" t="inlineStr">
@@ -4817,7 +4817,7 @@
       </c>
       <c r="G133" t="inlineStr">
         <is>
-          <t>17701</t>
+          <t>17702</t>
         </is>
       </c>
     </row>

</xml_diff>